<commit_message>
added and tested epros feature
</commit_message>
<xml_diff>
--- a/OUTPUT_DF/control_df.xlsx
+++ b/OUTPUT_DF/control_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>epros</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>covid</t>
         </is>
       </c>
@@ -479,6 +484,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -501,6 +509,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -523,6 +534,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -545,6 +559,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F5" t="n">
+        <v>44</v>
+      </c>
+      <c r="G5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -567,6 +584,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F6" t="n">
+        <v>70</v>
+      </c>
+      <c r="G6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -589,6 +609,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F7" t="n">
+        <v>36</v>
+      </c>
+      <c r="G7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -611,6 +634,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F8" t="n">
+        <v>33</v>
+      </c>
+      <c r="G8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -633,6 +659,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F9" t="n">
+        <v>31</v>
+      </c>
+      <c r="G9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -655,6 +684,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F10" t="n">
+        <v>29</v>
+      </c>
+      <c r="G10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -677,6 +709,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F11" t="n">
+        <v>28</v>
+      </c>
+      <c r="G11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -699,6 +734,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F12" t="n">
+        <v>14</v>
+      </c>
+      <c r="G12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -721,6 +759,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F13" t="n">
+        <v>14</v>
+      </c>
+      <c r="G13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -743,6 +784,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F14" t="n">
+        <v>39</v>
+      </c>
+      <c r="G14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -765,6 +809,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F15" t="n">
+        <v>30</v>
+      </c>
+      <c r="G15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -787,6 +834,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F16" t="n">
+        <v>29</v>
+      </c>
+      <c r="G16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -809,6 +859,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F17" t="n">
+        <v>45</v>
+      </c>
+      <c r="G17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -831,6 +884,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F18" t="n">
+        <v>35</v>
+      </c>
+      <c r="G18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -853,6 +909,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F19" t="n">
+        <v>17</v>
+      </c>
+      <c r="G19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -875,6 +934,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F20" t="n">
+        <v>21</v>
+      </c>
+      <c r="G20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -897,6 +959,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F21" t="n">
+        <v>10</v>
+      </c>
+      <c r="G21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -919,6 +984,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F22" t="n">
+        <v>24</v>
+      </c>
+      <c r="G22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -941,6 +1009,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F23" t="n">
+        <v>22</v>
+      </c>
+      <c r="G23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -963,6 +1034,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F24" t="n">
+        <v>51</v>
+      </c>
+      <c r="G24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -985,6 +1059,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F25" t="n">
+        <v>62</v>
+      </c>
+      <c r="G25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1007,6 +1084,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F26" t="n">
+        <v>67</v>
+      </c>
+      <c r="G26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1029,6 +1109,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F27" t="n">
+        <v>50</v>
+      </c>
+      <c r="G27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1051,6 +1134,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F28" t="n">
+        <v>15</v>
+      </c>
+      <c r="G28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1073,6 +1159,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F29" t="n">
+        <v>20</v>
+      </c>
+      <c r="G29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1095,6 +1184,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F30" t="n">
+        <v>11</v>
+      </c>
+      <c r="G30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1117,6 +1209,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F31" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1139,6 +1234,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F32" t="n">
+        <v>24</v>
+      </c>
+      <c r="G32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1161,6 +1259,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F33" t="n">
+        <v>45</v>
+      </c>
+      <c r="G33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1183,6 +1284,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F34" t="n">
+        <v>12</v>
+      </c>
+      <c r="G34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1205,6 +1309,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F35" t="n">
+        <v>8</v>
+      </c>
+      <c r="G35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1229,6 +1336,9 @@
       <c r="F36" t="n">
         <v>0</v>
       </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1249,6 +1359,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F37" t="n">
+        <v>8</v>
+      </c>
+      <c r="G37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1271,6 +1384,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F38" t="n">
+        <v>13</v>
+      </c>
+      <c r="G38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1293,6 +1409,9 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
+        <v>24</v>
+      </c>
+      <c r="G39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1315,6 +1434,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F40" t="n">
+        <v>22</v>
+      </c>
+      <c r="G40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1339,6 +1461,9 @@
       <c r="F41" t="n">
         <v>0</v>
       </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1359,6 +1484,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F42" t="n">
+        <v>23</v>
+      </c>
+      <c r="G42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1381,6 +1509,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F43" t="n">
+        <v>55</v>
+      </c>
+      <c r="G43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1403,6 +1534,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F44" t="n">
+        <v>1</v>
+      </c>
+      <c r="G44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1425,6 +1559,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F45" t="n">
+        <v>15</v>
+      </c>
+      <c r="G45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1447,6 +1584,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F46" t="n">
+        <v>16</v>
+      </c>
+      <c r="G46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1469,6 +1609,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1491,6 +1634,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F48" t="n">
+        <v>14</v>
+      </c>
+      <c r="G48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1513,6 +1659,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F49" t="n">
+        <v>19</v>
+      </c>
+      <c r="G49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1535,6 +1684,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F50" t="n">
+        <v>64</v>
+      </c>
+      <c r="G50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1557,6 +1709,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F51" t="n">
+        <v>38</v>
+      </c>
+      <c r="G51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1579,6 +1734,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F52" t="n">
+        <v>22</v>
+      </c>
+      <c r="G52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1601,6 +1759,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F53" t="n">
+        <v>29</v>
+      </c>
+      <c r="G53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1623,6 +1784,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F54" t="n">
+        <v>28</v>
+      </c>
+      <c r="G54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1645,6 +1809,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F55" t="n">
+        <v>33</v>
+      </c>
+      <c r="G55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1667,6 +1834,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F56" t="n">
+        <v>32</v>
+      </c>
+      <c r="G56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1689,6 +1859,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F57" t="n">
+        <v>29</v>
+      </c>
+      <c r="G57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1711,6 +1884,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F58" t="n">
+        <v>42</v>
+      </c>
+      <c r="G58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1733,6 +1909,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F59" t="n">
+        <v>39</v>
+      </c>
+      <c r="G59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1755,6 +1934,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F60" t="n">
+        <v>34</v>
+      </c>
+      <c r="G60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1777,6 +1959,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F61" t="n">
+        <v>31</v>
+      </c>
+      <c r="G61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1799,6 +1984,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F62" t="n">
+        <v>25</v>
+      </c>
+      <c r="G62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1821,6 +2009,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F63" t="n">
+        <v>22</v>
+      </c>
+      <c r="G63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1843,6 +2034,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F64" t="n">
+        <v>14</v>
+      </c>
+      <c r="G64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1865,6 +2059,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F65" t="n">
+        <v>31</v>
+      </c>
+      <c r="G65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1887,6 +2084,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F66" t="n">
+        <v>29</v>
+      </c>
+      <c r="G66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1909,6 +2109,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F67" t="n">
+        <v>13</v>
+      </c>
+      <c r="G67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1931,6 +2134,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F68" t="n">
+        <v>10</v>
+      </c>
+      <c r="G68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1953,6 +2159,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F69" t="n">
+        <v>63</v>
+      </c>
+      <c r="G69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1975,6 +2184,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F70" t="n">
+        <v>32</v>
+      </c>
+      <c r="G70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1997,6 +2209,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F71" t="n">
+        <v>43</v>
+      </c>
+      <c r="G71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2019,6 +2234,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F72" t="n">
+        <v>20</v>
+      </c>
+      <c r="G72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2041,6 +2259,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F73" t="n">
+        <v>16</v>
+      </c>
+      <c r="G73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2063,6 +2284,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F74" t="n">
+        <v>33</v>
+      </c>
+      <c r="G74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2085,6 +2309,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F75" t="n">
+        <v>30</v>
+      </c>
+      <c r="G75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2107,6 +2334,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F76" t="n">
+        <v>45</v>
+      </c>
+      <c r="G76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2129,6 +2359,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F77" t="n">
+        <v>57</v>
+      </c>
+      <c r="G77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2151,6 +2384,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F78" t="n">
+        <v>85</v>
+      </c>
+      <c r="G78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2173,6 +2409,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F79" t="n">
+        <v>24</v>
+      </c>
+      <c r="G79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2195,6 +2434,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F80" t="n">
+        <v>9</v>
+      </c>
+      <c r="G80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2217,6 +2459,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F81" t="n">
+        <v>39</v>
+      </c>
+      <c r="G81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2239,6 +2484,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F82" t="n">
+        <v>34</v>
+      </c>
+      <c r="G82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2261,6 +2509,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F83" t="n">
+        <v>22</v>
+      </c>
+      <c r="G83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2283,6 +2534,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F84" t="n">
+        <v>23</v>
+      </c>
+      <c r="G84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2305,6 +2559,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F85" t="n">
+        <v>13</v>
+      </c>
+      <c r="G85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2327,6 +2584,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F86" t="n">
+        <v>12</v>
+      </c>
+      <c r="G86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2351,6 +2611,9 @@
       <c r="F87" t="n">
         <v>0</v>
       </c>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2371,6 +2634,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
         <v>18.651428571</v>
       </c>
     </row>
@@ -2393,6 +2659,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F89" t="n">
+        <v>7</v>
+      </c>
+      <c r="G89" t="n">
         <v>43.98</v>
       </c>
     </row>
@@ -2415,6 +2684,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F90" t="n">
+        <v>11</v>
+      </c>
+      <c r="G90" t="n">
         <v>45.568571429</v>
       </c>
     </row>
@@ -2437,6 +2709,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
         <v>83.528571429</v>
       </c>
     </row>
@@ -2459,6 +2734,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2481,6 +2759,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F93" t="n">
+        <v>33</v>
+      </c>
+      <c r="G93" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2503,6 +2784,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F94" t="n">
+        <v>46</v>
+      </c>
+      <c r="G94" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2525,6 +2809,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F95" t="n">
+        <v>5</v>
+      </c>
+      <c r="G95" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2547,6 +2834,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F96" t="n">
+        <v>5</v>
+      </c>
+      <c r="G96" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2569,6 +2859,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F97" t="n">
+        <v>37</v>
+      </c>
+      <c r="G97" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2591,6 +2884,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F98" t="n">
+        <v>40</v>
+      </c>
+      <c r="G98" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2613,6 +2909,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F99" t="n">
+        <v>16</v>
+      </c>
+      <c r="G99" t="n">
         <v>76.84999999999999</v>
       </c>
     </row>
@@ -2635,6 +2934,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F100" t="n">
+        <v>17</v>
+      </c>
+      <c r="G100" t="n">
         <v>76.84999999999999</v>
       </c>
     </row>
@@ -2657,6 +2959,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F101" t="n">
+        <v>5</v>
+      </c>
+      <c r="G101" t="n">
         <v>75.264285714</v>
       </c>
     </row>
@@ -2679,6 +2984,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F102" t="n">
+        <v>44</v>
+      </c>
+      <c r="G102" t="n">
         <v>72.617142857</v>
       </c>
     </row>
@@ -2701,6 +3009,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F103" t="n">
+        <v>44</v>
+      </c>
+      <c r="G103" t="n">
         <v>72.22</v>
       </c>
     </row>
@@ -2723,6 +3034,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F104" t="n">
+        <v>34</v>
+      </c>
+      <c r="G104" t="n">
         <v>72.22</v>
       </c>
     </row>
@@ -2745,6 +3059,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F105" t="n">
+        <v>26</v>
+      </c>
+      <c r="G105" t="n">
         <v>51.85</v>
       </c>
     </row>
@@ -2767,6 +3084,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F106" t="n">
+        <v>24</v>
+      </c>
+      <c r="G106" t="n">
         <v>51.85</v>
       </c>
     </row>
@@ -2789,6 +3109,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F107" t="n">
+        <v>15</v>
+      </c>
+      <c r="G107" t="n">
         <v>50.264285714</v>
       </c>
     </row>
@@ -2811,6 +3134,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F108" t="n">
+        <v>3</v>
+      </c>
+      <c r="G108" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -2833,6 +3159,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F109" t="n">
+        <v>7</v>
+      </c>
+      <c r="G109" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -2855,6 +3184,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F110" t="n">
+        <v>42</v>
+      </c>
+      <c r="G110" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -2877,6 +3209,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F111" t="n">
+        <v>38</v>
+      </c>
+      <c r="G111" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -2899,6 +3234,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F112" t="n">
+        <v>31</v>
+      </c>
+      <c r="G112" t="n">
         <v>47.092857143</v>
       </c>
     </row>
@@ -2921,6 +3259,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F113" t="n">
+        <v>28</v>
+      </c>
+      <c r="G113" t="n">
         <v>48.15</v>
       </c>
     </row>
@@ -2943,6 +3284,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F114" t="n">
+        <v>13</v>
+      </c>
+      <c r="G114" t="n">
         <v>48.15</v>
       </c>
     </row>
@@ -2965,6 +3309,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F115" t="n">
+        <v>17</v>
+      </c>
+      <c r="G115" t="n">
         <v>48.015714286</v>
       </c>
     </row>
@@ -2987,6 +3334,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F116" t="n">
+        <v>24</v>
+      </c>
+      <c r="G116" t="n">
         <v>48.61</v>
       </c>
     </row>
@@ -3009,6 +3359,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F117" t="n">
+        <v>37</v>
+      </c>
+      <c r="G117" t="n">
         <v>48.61</v>
       </c>
     </row>
@@ -3031,6 +3384,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F118" t="n">
+        <v>48</v>
+      </c>
+      <c r="G118" t="n">
         <v>47.818571429</v>
       </c>
     </row>
@@ -3053,6 +3409,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F119" t="n">
+        <v>24</v>
+      </c>
+      <c r="G119" t="n">
         <v>49.54</v>
       </c>
     </row>
@@ -3075,6 +3434,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F120" t="n">
+        <v>17</v>
+      </c>
+      <c r="G120" t="n">
         <v>47.951428571</v>
       </c>
     </row>
@@ -3097,6 +3459,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F121" t="n">
+        <v>13</v>
+      </c>
+      <c r="G121" t="n">
         <v>45.568571429</v>
       </c>
     </row>
@@ -3119,6 +3484,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F122" t="n">
+        <v>28</v>
+      </c>
+      <c r="G122" t="n">
         <v>49.54</v>
       </c>
     </row>
@@ -3141,6 +3509,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F123" t="n">
+        <v>18</v>
+      </c>
+      <c r="G123" t="n">
         <v>62.037142857</v>
       </c>
     </row>
@@ -3163,6 +3534,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F124" t="n">
+        <v>26</v>
+      </c>
+      <c r="G124" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -3185,6 +3559,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F125" t="n">
+        <v>16</v>
+      </c>
+      <c r="G125" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -3207,6 +3584,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F126" t="n">
+        <v>32</v>
+      </c>
+      <c r="G126" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -3229,6 +3609,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F127" t="n">
+        <v>32</v>
+      </c>
+      <c r="G127" t="n">
         <v>77.642857143</v>
       </c>
     </row>
@@ -3251,6 +3634,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F128" t="n">
+        <v>53</v>
+      </c>
+      <c r="G128" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3273,6 +3659,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F129" t="n">
+        <v>43</v>
+      </c>
+      <c r="G129" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3295,6 +3684,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F130" t="n">
+        <v>71</v>
+      </c>
+      <c r="G130" t="n">
         <v>65.477142857</v>
       </c>
     </row>
@@ -3317,6 +3709,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F131" t="n">
+        <v>75</v>
+      </c>
+      <c r="G131" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3339,6 +3734,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F132" t="n">
+        <v>22</v>
+      </c>
+      <c r="G132" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3361,6 +3759,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F133" t="n">
+        <v>27</v>
+      </c>
+      <c r="G133" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3383,6 +3784,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F134" t="n">
+        <v>36</v>
+      </c>
+      <c r="G134" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3405,6 +3809,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F135" t="n">
+        <v>16</v>
+      </c>
+      <c r="G135" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3427,6 +3834,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F136" t="n">
+        <v>23</v>
+      </c>
+      <c r="G136" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3449,6 +3859,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F137" t="n">
+        <v>20</v>
+      </c>
+      <c r="G137" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3471,6 +3884,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F138" t="n">
+        <v>13</v>
+      </c>
+      <c r="G138" t="n">
         <v>60.19</v>
       </c>
     </row>
@@ -3493,6 +3909,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F139" t="n">
+        <v>13</v>
+      </c>
+      <c r="G139" t="n">
         <v>60.19</v>
       </c>
     </row>
@@ -3515,6 +3934,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F140" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="n">
         <v>64.552857143</v>
       </c>
     </row>
@@ -3537,6 +3959,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F141" t="n">
+        <v>9</v>
+      </c>
+      <c r="G141" t="n">
         <v>66.00714285700001</v>
       </c>
     </row>
@@ -3559,6 +3984,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F142" t="n">
+        <v>10</v>
+      </c>
+      <c r="G142" t="n">
         <v>65.61</v>
       </c>
     </row>
@@ -3581,6 +4009,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F143" t="n">
+        <v>14</v>
+      </c>
+      <c r="G143" t="n">
         <v>65.61</v>
       </c>
     </row>
@@ -3603,6 +4034,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F144" t="n">
+        <v>54</v>
+      </c>
+      <c r="G144" t="n">
         <v>69.577142857</v>
       </c>
     </row>
@@ -3625,6 +4059,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F145" t="n">
+        <v>58</v>
+      </c>
+      <c r="G145" t="n">
         <v>68.52</v>
       </c>
     </row>
@@ -3647,6 +4084,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F146" t="n">
+        <v>3</v>
+      </c>
+      <c r="G146" t="n">
         <v>74.471428571</v>
       </c>
     </row>
@@ -3669,6 +4109,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F147" t="n">
+        <v>5</v>
+      </c>
+      <c r="G147" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3691,6 +4134,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F148" t="n">
+        <v>46</v>
+      </c>
+      <c r="G148" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3713,6 +4159,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F149" t="n">
+        <v>38</v>
+      </c>
+      <c r="G149" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3735,6 +4184,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F150" t="n">
+        <v>4</v>
+      </c>
+      <c r="G150" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3757,6 +4209,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F151" t="n">
+        <v>14</v>
+      </c>
+      <c r="G151" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3779,6 +4234,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F152" t="n">
+        <v>16</v>
+      </c>
+      <c r="G152" t="n">
         <v>57.275714286</v>
       </c>
     </row>
@@ -3801,6 +4259,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F153" t="n">
+        <v>29</v>
+      </c>
+      <c r="G153" t="n">
         <v>54.63</v>
       </c>
     </row>
@@ -3823,6 +4284,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F154" t="n">
+        <v>35</v>
+      </c>
+      <c r="G154" t="n">
         <v>54.63</v>
       </c>
     </row>
@@ -3845,6 +4309,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F155" t="n">
+        <v>25</v>
+      </c>
+      <c r="G155" t="n">
         <v>54.63</v>
       </c>
     </row>
@@ -3867,6 +4334,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F156" t="n">
+        <v>51</v>
+      </c>
+      <c r="G156" t="n">
         <v>53.571428571</v>
       </c>
     </row>
@@ -3889,6 +4359,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F157" t="n">
+        <v>57</v>
+      </c>
+      <c r="G157" t="n">
         <v>47.22</v>
       </c>
     </row>
@@ -3911,6 +4384,9 @@
         <v>0.0101010101010101</v>
       </c>
       <c r="F158" t="n">
+        <v>13</v>
+      </c>
+      <c r="G158" t="n">
         <v>46.227142857</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added loyalty card (no good)
</commit_message>
<xml_diff>
--- a/OUTPUT_DF/control_df.xlsx
+++ b/OUTPUT_DF/control_df.xlsx
@@ -474,17 +474,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-0.000755070638773578</v>
+        <v>0.004034727766019211</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -499,17 +499,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>-0.003652486835248147</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F3" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -524,17 +524,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-0.0023005887912552</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -549,17 +549,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.003101670918833577</v>
+        <v>-0.006235258055066545</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F5" t="n">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -574,17 +574,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.004697797155616752</v>
+        <v>-0.00968659940641187</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F6" t="n">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -599,17 +599,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.0003789571852221888</v>
+        <v>0.01395029322421881</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F7" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -624,17 +624,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.002117303653251161</v>
+        <v>0.01254757352393429</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F8" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -649,17 +649,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.002101627672492546</v>
+        <v>0.00450013546274506</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F9" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -674,17 +674,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.002172880431713447</v>
+        <v>0.008829448487061124</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F10" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -699,17 +699,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.0001543945178605364</v>
+        <v>0.03521333901604005</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F11" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -724,17 +724,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.0004813968263644681</v>
+        <v>0.02950060593747095</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F12" t="n">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -749,17 +749,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.001464672994755865</v>
+        <v>0.03681799175613665</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F13" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -774,17 +774,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.01643366013260521</v>
+        <v>0.04447319895146391</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F14" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -799,17 +799,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.01550349288691184</v>
+        <v>0.05358513318660785</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F15" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -824,14 +824,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.009563930640143766</v>
+        <v>0.04259081657257695</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F16" t="n">
         <v>29</v>
@@ -849,17 +849,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.01397933308998778</v>
+        <v>0.02198908082029977</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F17" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -874,17 +874,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.01386305176373523</v>
+        <v>0.01130355643973088</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F18" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -899,17 +899,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.003110094580476946</v>
+        <v>0.01556871373029011</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F19" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -924,17 +924,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.009724221219946672</v>
+        <v>0.02555939954859926</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F20" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -949,17 +949,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.00352083912584532</v>
+        <v>0.008027154973763795</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F21" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -974,17 +974,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.008153204471490342</v>
+        <v>0.01867961453903383</v>
       </c>
       <c r="E22" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F22" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -999,17 +999,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.007937631396755214</v>
+        <v>0.05760112085918486</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F23" t="n">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -1024,17 +1024,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.01698608418270394</v>
+        <v>0.07484688568677077</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F24" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1049,17 +1049,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.01308072829589028</v>
+        <v>0.04626323537411289</v>
       </c>
       <c r="E25" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F25" t="n">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -1074,17 +1074,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.01510769907042788</v>
+        <v>0.05437264215409243</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F26" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -1099,17 +1099,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.01222410353511274</v>
+        <v>0.05064101736794163</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F27" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1124,17 +1124,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.003414730187523015</v>
+        <v>0.01818067777897367</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F28" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -1149,17 +1149,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.02226962823471006</v>
+        <v>0.01388979310241541</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F29" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1174,17 +1174,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.003535126581084022</v>
+        <v>0.01367927032789854</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F30" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -1199,17 +1199,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.002637748489022921</v>
+        <v>0.01456377378651633</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -1224,17 +1224,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>-0.01485425883056215</v>
+        <v>0.003047253383390853</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F32" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1249,17 +1249,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.02288468778394557</v>
+        <v>0.01867474951167743</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F33" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -1274,17 +1274,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.01148581168291831</v>
+        <v>0.004045152543858919</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F34" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -1299,14 +1299,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.01033465832326398</v>
+        <v>0.01843410564893042</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F35" t="n">
         <v>8</v>
@@ -1324,17 +1324,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.01041982759822606</v>
+        <v>0.01579117601220473</v>
       </c>
       <c r="E36" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
@@ -1349,17 +1349,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.01491878149848453</v>
+        <v>0.02271937350701201</v>
       </c>
       <c r="E37" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F37" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -1374,17 +1374,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.01043451825257207</v>
+        <v>0.01962757215821579</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F38" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -1399,17 +1399,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.007023504440674107</v>
+        <v>0.01937221827473221</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F39" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -1424,17 +1424,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.007820833146087103</v>
+        <v>0.03248660847614245</v>
       </c>
       <c r="E40" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F40" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -1449,17 +1449,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.008690585191936122</v>
+        <v>0.03516925559223718</v>
       </c>
       <c r="E41" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -1474,17 +1474,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.01055448488542959</v>
+        <v>0.03309894677845424</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F42" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
@@ -1499,17 +1499,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.01206092087226486</v>
+        <v>0.0285169492581372</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F43" t="n">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
@@ -1524,17 +1524,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.009691637397433317</v>
+        <v>0.01070836387313437</v>
       </c>
       <c r="E44" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -1549,17 +1549,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.01089774698983685</v>
+        <v>0.007875574967370414</v>
       </c>
       <c r="E45" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F45" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -1574,17 +1574,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.008684005781253683</v>
+        <v>-0.002289178648226958</v>
       </c>
       <c r="E46" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F46" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -1599,17 +1599,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.004505032532613161</v>
+        <v>0.01522342873919984</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F47" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
@@ -1624,17 +1624,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.009789435764383091</v>
+        <v>0.01850686253593583</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F48" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -1649,17 +1649,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.007896089336321582</v>
+        <v>0.01111170385397318</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F49" t="n">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
@@ -1674,17 +1674,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.01963257588880598</v>
+        <v>0.01002225445216644</v>
       </c>
       <c r="E50" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F50" t="n">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
@@ -1699,17 +1699,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.007825310557779599</v>
+        <v>0.01137675501299126</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F51" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -1724,17 +1724,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.005830171586509581</v>
+        <v>0.007347829316574565</v>
       </c>
       <c r="E52" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F52" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -1749,17 +1749,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.00437113444692316</v>
+        <v>0.004434293954786269</v>
       </c>
       <c r="E53" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F53" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
@@ -1774,17 +1774,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.002545820485515261</v>
+        <v>0.004733245539153396</v>
       </c>
       <c r="E54" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F54" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
@@ -1799,17 +1799,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.003197490231616198</v>
+        <v>0.00278185777810078</v>
       </c>
       <c r="E55" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F55" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="G55" t="n">
         <v>0</v>
@@ -1824,17 +1824,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.005302044169953019</v>
+        <v>0.007268932406056768</v>
       </c>
       <c r="E56" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F56" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
@@ -1849,17 +1849,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.005704508042787212</v>
+        <v>0.0005635901970911153</v>
       </c>
       <c r="E57" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F57" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
@@ -1874,17 +1874,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.009090172517134055</v>
+        <v>0.001360767750296443</v>
       </c>
       <c r="E58" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F58" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -1899,17 +1899,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.007606325146227353</v>
+        <v>0.006579608802793816</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F59" t="n">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -1924,17 +1924,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.007307142415619871</v>
+        <v>0.009583862130579197</v>
       </c>
       <c r="E60" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F60" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G60" t="n">
         <v>0</v>
@@ -1949,17 +1949,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.006653400945457578</v>
+        <v>0.003561744653356064</v>
       </c>
       <c r="E61" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F61" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -1974,17 +1974,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.005690430348873847</v>
+        <v>0.005540539488117736</v>
       </c>
       <c r="E62" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F62" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
         <v>0</v>
@@ -1999,17 +1999,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.005448453933323168</v>
+        <v>0.01743319897094744</v>
       </c>
       <c r="E63" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F63" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
@@ -2024,17 +2024,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.007200075498693608</v>
+        <v>0.008164500434874924</v>
       </c>
       <c r="E64" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F64" t="n">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
@@ -2049,17 +2049,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.009782353393971382</v>
+        <v>0.01073016343231211</v>
       </c>
       <c r="E65" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F65" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2074,17 +2074,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.01344714076958524</v>
+        <v>0.0169149173029911</v>
       </c>
       <c r="E66" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F66" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
@@ -2099,17 +2099,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.01080954111593122</v>
+        <v>0.01663740438499015</v>
       </c>
       <c r="E67" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F67" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
@@ -2124,17 +2124,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.007825440334571283</v>
+        <v>0.01256307036933456</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F68" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
@@ -2149,17 +2149,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.01378572695054878</v>
+        <v>0.004903710417211724</v>
       </c>
       <c r="E69" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F69" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="G69" t="n">
         <v>0</v>
@@ -2174,17 +2174,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.007152598140873686</v>
+        <v>0.0001242889194008451</v>
       </c>
       <c r="E70" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F70" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -2199,17 +2199,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.01569393226003413</v>
+        <v>-0.002335413003600234</v>
       </c>
       <c r="E71" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F71" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
         <v>0</v>
@@ -2224,17 +2224,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.01488047603857827</v>
+        <v>0.009262530228667635</v>
       </c>
       <c r="E72" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F72" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
@@ -2249,17 +2249,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.01079766790691434</v>
+        <v>0.0008106444775059619</v>
       </c>
       <c r="E73" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="F73" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
@@ -2274,17 +2274,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.009582232973597298</v>
+        <v>0.01058680715270364</v>
       </c>
       <c r="E74" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F74" t="n">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
@@ -2299,17 +2299,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.01790255139203105</v>
+        <v>0.01569481807676036</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="F75" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G75" t="n">
         <v>0</v>
@@ -2324,17 +2324,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.01386153067190398</v>
+        <v>0.03681704102737446</v>
       </c>
       <c r="E76" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="F76" t="n">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="G76" t="n">
         <v>0</v>
@@ -2349,17 +2349,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.01400517204100869</v>
+        <v>0.05231892312623063</v>
       </c>
       <c r="E77" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F77" t="n">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G77" t="n">
         <v>0</v>
@@ -2374,17 +2374,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.0143223944506718</v>
+        <v>0.04026561908612234</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F78" t="n">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="G78" t="n">
         <v>0</v>
@@ -2399,17 +2399,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.01179564814916764</v>
+        <v>0.03194262104914274</v>
       </c>
       <c r="E79" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F79" t="n">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G79" t="n">
         <v>0</v>
@@ -2424,17 +2424,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.006542962425941732</v>
+        <v>0.002828196590327276</v>
       </c>
       <c r="E80" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F80" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
@@ -2449,17 +2449,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.02064152064965953</v>
+        <v>0.005642551149875327</v>
       </c>
       <c r="E81" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F81" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="G81" t="n">
         <v>0</v>
@@ -2474,17 +2474,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.01064941868386761</v>
+        <v>0.00965565121936794</v>
       </c>
       <c r="E82" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F82" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G82" t="n">
         <v>0</v>
@@ -2499,17 +2499,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.008371128671742719</v>
+        <v>0.004912892396111082</v>
       </c>
       <c r="E83" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F83" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="G83" t="n">
         <v>0</v>
@@ -2524,17 +2524,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.006269717046145053</v>
+        <v>0.0005888132455438922</v>
       </c>
       <c r="E84" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="F84" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G84" t="n">
         <v>0</v>
@@ -2549,17 +2549,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0.00318567247486958</v>
+        <v>-0.004260287744343218</v>
       </c>
       <c r="E85" t="n">
-        <v>0.0101010101010101</v>
+        <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G85" t="n">
         <v>0</v>
@@ -2574,17 +2574,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.0002767931389714694</v>
+        <v>0.001189007667551305</v>
       </c>
       <c r="E86" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F86" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G86" t="n">
         <v>0</v>
@@ -2599,17 +2599,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>-0.0002869853509251468</v>
+        <v>0.006939172453089029</v>
       </c>
       <c r="E87" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G87" t="n">
         <v>0</v>
@@ -2624,14 +2624,14 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>-0.0002720456314996333</v>
+        <v>-3.107464370894401e-05</v>
       </c>
       <c r="E88" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -2649,17 +2649,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0.003571348907385504</v>
+        <v>-0.002731570822729588</v>
       </c>
       <c r="E89" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="F89" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G89" t="n">
         <v>43.98</v>
@@ -2674,17 +2674,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.002331480227889832</v>
+        <v>0.008991972697265985</v>
       </c>
       <c r="E90" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="F90" t="n">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G90" t="n">
         <v>45.568571429</v>
@@ -2699,17 +2699,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>-3.527607193329877e-05</v>
+        <v>-0.008152364194303978</v>
       </c>
       <c r="E91" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="F91" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G91" t="n">
         <v>83.528571429</v>
@@ -2724,17 +2724,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>-0.0005569389141133346</v>
+        <v>0.002584094415187901</v>
       </c>
       <c r="E92" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="G92" t="n">
         <v>87.95999999999999</v>
@@ -2749,17 +2749,17 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.003639806497956753</v>
+        <v>0.002476541124255196</v>
       </c>
       <c r="E93" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.02380952380952381</v>
       </c>
       <c r="F93" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G93" t="n">
         <v>87.95999999999999</v>
@@ -2774,17 +2774,17 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.004696267324961371</v>
+        <v>0.002943781648588592</v>
       </c>
       <c r="E94" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.02380952380952381</v>
       </c>
       <c r="F94" t="n">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G94" t="n">
         <v>87.95999999999999</v>
@@ -2799,17 +2799,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0.002267929313189486</v>
+        <v>-0.01900442560897979</v>
       </c>
       <c r="E95" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="F95" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G95" t="n">
         <v>87.95999999999999</v>
@@ -2824,17 +2824,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0.001299394348995923</v>
+        <v>-0.01562154577015635</v>
       </c>
       <c r="E96" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.03571428571428571</v>
       </c>
       <c r="F96" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G96" t="n">
         <v>87.95999999999999</v>
@@ -2849,17 +2849,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0.00212934198648457</v>
+        <v>-0.02023764422383352</v>
       </c>
       <c r="E97" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.02380952380952381</v>
       </c>
       <c r="F97" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G97" t="n">
         <v>87.95999999999999</v>
@@ -2874,17 +2874,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0.001377083796975972</v>
+        <v>-0.0155398519556115</v>
       </c>
       <c r="E98" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="F98" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G98" t="n">
         <v>87.95999999999999</v>
@@ -2899,17 +2899,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0.002981657044506518</v>
+        <v>-0.004986784762649699</v>
       </c>
       <c r="E99" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="F99" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G99" t="n">
         <v>76.84999999999999</v>
@@ -2924,17 +2924,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.001890622948251248</v>
+        <v>0.0002354810938828598</v>
       </c>
       <c r="E100" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F100" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G100" t="n">
         <v>76.84999999999999</v>
@@ -2949,17 +2949,17 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>-6.482993427956871e-05</v>
+        <v>0.008746980757410669</v>
       </c>
       <c r="E101" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="F101" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="G101" t="n">
         <v>75.264285714</v>
@@ -2974,17 +2974,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0.01443306260835856</v>
+        <v>0.003100039220989352</v>
       </c>
       <c r="E102" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1071428571428571</v>
       </c>
       <c r="F102" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G102" t="n">
         <v>72.617142857</v>
@@ -2999,17 +2999,17 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0.005197993886685044</v>
+        <v>0.000480468173680484</v>
       </c>
       <c r="E103" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F103" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="G103" t="n">
         <v>72.22</v>
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0.001983272616301942</v>
+        <v>0.00538699032764811</v>
       </c>
       <c r="E104" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F104" t="n">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="G104" t="n">
         <v>72.22</v>
@@ -3049,17 +3049,17 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0.0001411042877328555</v>
+        <v>0.01433111688781056</v>
       </c>
       <c r="E105" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F105" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G105" t="n">
         <v>51.85</v>
@@ -3074,17 +3074,17 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0.0002904243942506539</v>
+        <v>0.009777546357939915</v>
       </c>
       <c r="E106" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F106" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G106" t="n">
         <v>51.85</v>
@@ -3099,17 +3099,17 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>-0.0008273607067611426</v>
+        <v>0.008296424136416784</v>
       </c>
       <c r="E107" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F107" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G107" t="n">
         <v>50.264285714</v>
@@ -3124,17 +3124,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>-0.001414245312102238</v>
+        <v>0.004779554082304271</v>
       </c>
       <c r="E108" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F108" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G108" t="n">
         <v>46.3</v>
@@ -3149,17 +3149,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>-0.0007213864818561709</v>
+        <v>0.01022652029850562</v>
       </c>
       <c r="E109" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F109" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G109" t="n">
         <v>46.3</v>
@@ -3174,17 +3174,17 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0.004376896017556402</v>
+        <v>0.01147196410410921</v>
       </c>
       <c r="E110" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F110" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="G110" t="n">
         <v>46.3</v>
@@ -3199,17 +3199,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0.002639431139571133</v>
+        <v>0.01495171420750315</v>
       </c>
       <c r="E111" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F111" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="G111" t="n">
         <v>46.3</v>
@@ -3224,17 +3224,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0.0007634974224028804</v>
+        <v>0.0176738758334347</v>
       </c>
       <c r="E112" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F112" t="n">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="G112" t="n">
         <v>47.092857143</v>
@@ -3249,17 +3249,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0.002503560850889579</v>
+        <v>0.01241238820614243</v>
       </c>
       <c r="E113" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F113" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G113" t="n">
         <v>48.15</v>
@@ -3274,17 +3274,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>0.005358659026915535</v>
+        <v>0.01829190865080234</v>
       </c>
       <c r="E114" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F114" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G114" t="n">
         <v>48.15</v>
@@ -3299,17 +3299,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0.002284018263936385</v>
+        <v>0.02271122930368995</v>
       </c>
       <c r="E115" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F115" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="G115" t="n">
         <v>48.015714286</v>
@@ -3324,17 +3324,17 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>0.00240019628538921</v>
+        <v>0.02483060736198625</v>
       </c>
       <c r="E116" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F116" t="n">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="G116" t="n">
         <v>48.61</v>
@@ -3349,17 +3349,17 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>-0.001952612326819562</v>
+        <v>0.03025426912248452</v>
       </c>
       <c r="E117" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F117" t="n">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="G117" t="n">
         <v>48.61</v>
@@ -3374,17 +3374,17 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0.008841609249927529</v>
+        <v>0.05413258065632754</v>
       </c>
       <c r="E118" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F118" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G118" t="n">
         <v>47.818571429</v>
@@ -3399,17 +3399,17 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0.006341762531922348</v>
+        <v>0.04843081824170002</v>
       </c>
       <c r="E119" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F119" t="n">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="G119" t="n">
         <v>49.54</v>
@@ -3424,17 +3424,17 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0.004039360578522472</v>
+        <v>0.04135594063929158</v>
       </c>
       <c r="E120" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F120" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G120" t="n">
         <v>47.951428571</v>
@@ -3449,17 +3449,17 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>0.003742992946637556</v>
+        <v>0.02115944543274189</v>
       </c>
       <c r="E121" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F121" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="G121" t="n">
         <v>45.568571429</v>
@@ -3474,17 +3474,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0.008440493188665873</v>
+        <v>0.01508423014601739</v>
       </c>
       <c r="E122" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="F122" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G122" t="n">
         <v>49.54</v>
@@ -3499,17 +3499,17 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0.008919047414160877</v>
+        <v>0.00443738911121695</v>
       </c>
       <c r="E123" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F123" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G123" t="n">
         <v>62.037142857</v>
@@ -3524,17 +3524,17 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>0.01172893309590481</v>
+        <v>-0.002663539907622035</v>
       </c>
       <c r="E124" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F124" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="G124" t="n">
         <v>78.7</v>
@@ -3549,17 +3549,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0.005920833237787753</v>
+        <v>0.001827423728256047</v>
       </c>
       <c r="E125" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.119047619047619</v>
       </c>
       <c r="F125" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G125" t="n">
         <v>78.7</v>
@@ -3574,17 +3574,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>0.005286479339530283</v>
+        <v>0.003647451381532653</v>
       </c>
       <c r="E126" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F126" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="G126" t="n">
         <v>78.7</v>
@@ -3599,17 +3599,17 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0.005556197629816253</v>
+        <v>0.01814484409510526</v>
       </c>
       <c r="E127" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.130952380952381</v>
       </c>
       <c r="F127" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="G127" t="n">
         <v>77.642857143</v>
@@ -3624,17 +3624,17 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>0.01233426019797245</v>
+        <v>0.04219486836176774</v>
       </c>
       <c r="E128" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F128" t="n">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="G128" t="n">
         <v>75</v>
@@ -3649,17 +3649,17 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>0.008415870828738934</v>
+        <v>0.06597945623659511</v>
       </c>
       <c r="E129" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F129" t="n">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="G129" t="n">
         <v>75</v>
@@ -3674,17 +3674,17 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>0.009680382819717856</v>
+        <v>0.0480313805725991</v>
       </c>
       <c r="E130" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F130" t="n">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="G130" t="n">
         <v>65.477142857</v>
@@ -3699,17 +3699,17 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>0.01147904732748661</v>
+        <v>0.03262586036263665</v>
       </c>
       <c r="E131" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F131" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G131" t="n">
         <v>63.89</v>
@@ -3724,17 +3724,17 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>0.006436357158480325</v>
+        <v>0.02491272382368888</v>
       </c>
       <c r="E132" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F132" t="n">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G132" t="n">
         <v>63.89</v>
@@ -3749,17 +3749,17 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>0.005210144203667675</v>
+        <v>0.01182863617724419</v>
       </c>
       <c r="E133" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F133" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G133" t="n">
         <v>63.89</v>
@@ -3774,17 +3774,17 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>0.01832145399187561</v>
+        <v>0.01245684324353774</v>
       </c>
       <c r="E134" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="F134" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="G134" t="n">
         <v>63.89</v>
@@ -3799,17 +3799,17 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0.007474876791037421</v>
+        <v>0.0148783859449537</v>
       </c>
       <c r="E135" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F135" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G135" t="n">
         <v>63.89</v>
@@ -3824,17 +3824,17 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>0.004663629770938988</v>
+        <v>0.01376802809051519</v>
       </c>
       <c r="E136" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F136" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G136" t="n">
         <v>63.89</v>
@@ -3849,17 +3849,17 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>0.0005189010792343414</v>
+        <v>0.01444338249507196</v>
       </c>
       <c r="E137" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F137" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G137" t="n">
         <v>63.89</v>
@@ -3874,17 +3874,17 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0.007139646659534228</v>
+        <v>0.01389728731213731</v>
       </c>
       <c r="E138" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F138" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G138" t="n">
         <v>60.19</v>
@@ -3899,17 +3899,17 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>0.00161959034616894</v>
+        <v>0.01502864744202661</v>
       </c>
       <c r="E139" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F139" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G139" t="n">
         <v>60.19</v>
@@ -3924,14 +3924,14 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>-0.001776756973831556</v>
+        <v>0.01563125726841101</v>
       </c>
       <c r="E140" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F140" t="n">
         <v>0</v>
@@ -3949,17 +3949,17 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0.002178137166467781</v>
+        <v>0.018015076877317</v>
       </c>
       <c r="E141" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F141" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G141" t="n">
         <v>66.00714285700001</v>
@@ -3974,17 +3974,17 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>-0.001029795664263842</v>
+        <v>0.02581236773749168</v>
       </c>
       <c r="E142" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F142" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G142" t="n">
         <v>65.61</v>
@@ -3999,17 +3999,17 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>-0.0007323480876772109</v>
+        <v>0.0230118592788356</v>
       </c>
       <c r="E143" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F143" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G143" t="n">
         <v>65.61</v>
@@ -4024,17 +4024,17 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>0.006137471391615688</v>
+        <v>0.01594786518951187</v>
       </c>
       <c r="E144" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F144" t="n">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="G144" t="n">
         <v>69.577142857</v>
@@ -4049,17 +4049,17 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>0.005941977381314426</v>
+        <v>0.02809851251502965</v>
       </c>
       <c r="E145" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F145" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G145" t="n">
         <v>68.52</v>
@@ -4074,17 +4074,17 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>-0.00039966739306927</v>
+        <v>0.001800671236309095</v>
       </c>
       <c r="E146" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F146" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="G146" t="n">
         <v>74.471428571</v>
@@ -4099,17 +4099,17 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>-0.000994432806304177</v>
+        <v>-0.0004506748932470333</v>
       </c>
       <c r="E147" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F147" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="G147" t="n">
         <v>75</v>
@@ -4124,17 +4124,17 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0.00293556569940153</v>
+        <v>0.01737311568163392</v>
       </c>
       <c r="E148" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F148" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G148" t="n">
         <v>75</v>
@@ -4149,17 +4149,17 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>0.003769481709610888</v>
+        <v>0.01200811627223967</v>
       </c>
       <c r="E149" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F149" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G149" t="n">
         <v>75</v>
@@ -4174,17 +4174,17 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>0.00599894169667809</v>
+        <v>0.003474428050545215</v>
       </c>
       <c r="E150" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F150" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G150" t="n">
         <v>63.89</v>
@@ -4199,17 +4199,17 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0.004807201288955304</v>
+        <v>-0.002051826131524507</v>
       </c>
       <c r="E151" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F151" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G151" t="n">
         <v>63.89</v>
@@ -4224,17 +4224,17 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0.005146356503197043</v>
+        <v>0.007689060222708656</v>
       </c>
       <c r="E152" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F152" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G152" t="n">
         <v>57.275714286</v>
@@ -4249,17 +4249,17 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>0.01611699799204318</v>
+        <v>0.01210186438738531</v>
       </c>
       <c r="E153" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F153" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="G153" t="n">
         <v>54.63</v>
@@ -4274,17 +4274,17 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>0.008065375571913631</v>
+        <v>0.009578065752443458</v>
       </c>
       <c r="E154" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F154" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G154" t="n">
         <v>54.63</v>
@@ -4299,17 +4299,17 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>0.004756968971478957</v>
+        <v>0.006131251934973499</v>
       </c>
       <c r="E155" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F155" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G155" t="n">
         <v>54.63</v>
@@ -4324,17 +4324,17 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0.006471816106636408</v>
+        <v>0.01149321151501131</v>
       </c>
       <c r="E156" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F156" t="n">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="G156" t="n">
         <v>53.571428571</v>
@@ -4349,17 +4349,17 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>0.003759315811925113</v>
+        <v>0.00267705192264671</v>
       </c>
       <c r="E157" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F157" t="n">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="G157" t="n">
         <v>47.22</v>
@@ -4374,17 +4374,17 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>fast_duck</t>
+          <t>precious_liquid</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>0.001598669572276741</v>
+        <v>0.005879027449751367</v>
       </c>
       <c r="E158" t="n">
-        <v>0.0101010101010101</v>
+        <v>0.1547619047619048</v>
       </c>
       <c r="F158" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G158" t="n">
         <v>46.227142857</v>

</xml_diff>

<commit_message>
off trade feature implemented and tested
</commit_message>
<xml_diff>
--- a/OUTPUT_DF/control_df.xlsx
+++ b/OUTPUT_DF/control_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:H158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>off_trade_visibility</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>covid</t>
         </is>
       </c>
@@ -487,6 +492,9 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
+        <v>11</v>
+      </c>
+      <c r="H2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -512,6 +520,9 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -537,6 +548,9 @@
         <v>3</v>
       </c>
       <c r="G4" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -562,6 +576,9 @@
         <v>15</v>
       </c>
       <c r="G5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -587,6 +604,9 @@
         <v>18</v>
       </c>
       <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -612,6 +632,9 @@
         <v>4</v>
       </c>
       <c r="G7" t="n">
+        <v>13</v>
+      </c>
+      <c r="H7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -637,6 +660,9 @@
         <v>3</v>
       </c>
       <c r="G8" t="n">
+        <v>9</v>
+      </c>
+      <c r="H8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -662,6 +688,9 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -687,6 +716,9 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -712,6 +744,9 @@
         <v>14</v>
       </c>
       <c r="G11" t="n">
+        <v>18</v>
+      </c>
+      <c r="H11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -737,6 +772,9 @@
         <v>38</v>
       </c>
       <c r="G12" t="n">
+        <v>36</v>
+      </c>
+      <c r="H12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -762,6 +800,9 @@
         <v>32</v>
       </c>
       <c r="G13" t="n">
+        <v>21</v>
+      </c>
+      <c r="H13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -787,6 +828,9 @@
         <v>45</v>
       </c>
       <c r="G14" t="n">
+        <v>18</v>
+      </c>
+      <c r="H14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -812,6 +856,9 @@
         <v>34</v>
       </c>
       <c r="G15" t="n">
+        <v>8</v>
+      </c>
+      <c r="H15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -837,6 +884,9 @@
         <v>29</v>
       </c>
       <c r="G16" t="n">
+        <v>16</v>
+      </c>
+      <c r="H16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -862,6 +912,9 @@
         <v>1</v>
       </c>
       <c r="G17" t="n">
+        <v>5</v>
+      </c>
+      <c r="H17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -887,6 +940,9 @@
         <v>5</v>
       </c>
       <c r="G18" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -912,6 +968,9 @@
         <v>3</v>
       </c>
       <c r="G19" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -937,6 +996,9 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
+        <v>12</v>
+      </c>
+      <c r="H20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -962,6 +1024,9 @@
         <v>14</v>
       </c>
       <c r="G21" t="n">
+        <v>18</v>
+      </c>
+      <c r="H21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -987,6 +1052,9 @@
         <v>13</v>
       </c>
       <c r="G22" t="n">
+        <v>14</v>
+      </c>
+      <c r="H22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1012,6 +1080,9 @@
         <v>48</v>
       </c>
       <c r="G23" t="n">
+        <v>20</v>
+      </c>
+      <c r="H23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1037,6 +1108,9 @@
         <v>35</v>
       </c>
       <c r="G24" t="n">
+        <v>28</v>
+      </c>
+      <c r="H24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1062,6 +1136,9 @@
         <v>79</v>
       </c>
       <c r="G25" t="n">
+        <v>46</v>
+      </c>
+      <c r="H25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1087,6 +1164,9 @@
         <v>69</v>
       </c>
       <c r="G26" t="n">
+        <v>68</v>
+      </c>
+      <c r="H26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1112,6 +1192,9 @@
         <v>44</v>
       </c>
       <c r="G27" t="n">
+        <v>57</v>
+      </c>
+      <c r="H27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1137,6 +1220,9 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
+        <v>35</v>
+      </c>
+      <c r="H28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1162,6 +1248,9 @@
         <v>0</v>
       </c>
       <c r="G29" t="n">
+        <v>19</v>
+      </c>
+      <c r="H29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1187,6 +1276,9 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
+        <v>14</v>
+      </c>
+      <c r="H30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1212,6 +1304,9 @@
         <v>0</v>
       </c>
       <c r="G31" t="n">
+        <v>12</v>
+      </c>
+      <c r="H31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1237,6 +1332,9 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
+        <v>14</v>
+      </c>
+      <c r="H32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1262,6 +1360,9 @@
         <v>4</v>
       </c>
       <c r="G33" t="n">
+        <v>10</v>
+      </c>
+      <c r="H33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1287,6 +1388,9 @@
         <v>10</v>
       </c>
       <c r="G34" t="n">
+        <v>15</v>
+      </c>
+      <c r="H34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1312,6 +1416,9 @@
         <v>8</v>
       </c>
       <c r="G35" t="n">
+        <v>16</v>
+      </c>
+      <c r="H35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1337,6 +1444,9 @@
         <v>5</v>
       </c>
       <c r="G36" t="n">
+        <v>13</v>
+      </c>
+      <c r="H36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1362,6 +1472,9 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
+        <v>14</v>
+      </c>
+      <c r="H37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1387,6 +1500,9 @@
         <v>2</v>
       </c>
       <c r="G38" t="n">
+        <v>16</v>
+      </c>
+      <c r="H38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1412,6 +1528,9 @@
         <v>6</v>
       </c>
       <c r="G39" t="n">
+        <v>15</v>
+      </c>
+      <c r="H39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1437,6 +1556,9 @@
         <v>23</v>
       </c>
       <c r="G40" t="n">
+        <v>14</v>
+      </c>
+      <c r="H40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1462,6 +1584,9 @@
         <v>36</v>
       </c>
       <c r="G41" t="n">
+        <v>21</v>
+      </c>
+      <c r="H41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1487,6 +1612,9 @@
         <v>35</v>
       </c>
       <c r="G42" t="n">
+        <v>13</v>
+      </c>
+      <c r="H42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1512,6 +1640,9 @@
         <v>9</v>
       </c>
       <c r="G43" t="n">
+        <v>14</v>
+      </c>
+      <c r="H43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1537,6 +1668,9 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
+        <v>14</v>
+      </c>
+      <c r="H44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1562,6 +1696,9 @@
         <v>0</v>
       </c>
       <c r="G45" t="n">
+        <v>9</v>
+      </c>
+      <c r="H45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1587,6 +1724,9 @@
         <v>9</v>
       </c>
       <c r="G46" t="n">
+        <v>10</v>
+      </c>
+      <c r="H46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1612,6 +1752,9 @@
         <v>24</v>
       </c>
       <c r="G47" t="n">
+        <v>7</v>
+      </c>
+      <c r="H47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1637,6 +1780,9 @@
         <v>23</v>
       </c>
       <c r="G48" t="n">
+        <v>11</v>
+      </c>
+      <c r="H48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1662,6 +1808,9 @@
         <v>33</v>
       </c>
       <c r="G49" t="n">
+        <v>6</v>
+      </c>
+      <c r="H49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1687,6 +1836,9 @@
         <v>30</v>
       </c>
       <c r="G50" t="n">
+        <v>7</v>
+      </c>
+      <c r="H50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1712,6 +1864,9 @@
         <v>12</v>
       </c>
       <c r="G51" t="n">
+        <v>9</v>
+      </c>
+      <c r="H51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1737,6 +1892,9 @@
         <v>4</v>
       </c>
       <c r="G52" t="n">
+        <v>7</v>
+      </c>
+      <c r="H52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1762,6 +1920,9 @@
         <v>1</v>
       </c>
       <c r="G53" t="n">
+        <v>7</v>
+      </c>
+      <c r="H53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1787,6 +1948,9 @@
         <v>6</v>
       </c>
       <c r="G54" t="n">
+        <v>6</v>
+      </c>
+      <c r="H54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1812,6 +1976,9 @@
         <v>7</v>
       </c>
       <c r="G55" t="n">
+        <v>7</v>
+      </c>
+      <c r="H55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1837,6 +2004,9 @@
         <v>5</v>
       </c>
       <c r="G56" t="n">
+        <v>6</v>
+      </c>
+      <c r="H56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1862,6 +2032,9 @@
         <v>0</v>
       </c>
       <c r="G57" t="n">
+        <v>6</v>
+      </c>
+      <c r="H57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1887,6 +2060,9 @@
         <v>0</v>
       </c>
       <c r="G58" t="n">
+        <v>8</v>
+      </c>
+      <c r="H58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1912,6 +2088,9 @@
         <v>3</v>
       </c>
       <c r="G59" t="n">
+        <v>5</v>
+      </c>
+      <c r="H59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1937,6 +2116,9 @@
         <v>2</v>
       </c>
       <c r="G60" t="n">
+        <v>4</v>
+      </c>
+      <c r="H60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1962,6 +2144,9 @@
         <v>0</v>
       </c>
       <c r="G61" t="n">
+        <v>5</v>
+      </c>
+      <c r="H61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1987,6 +2172,9 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
+        <v>4</v>
+      </c>
+      <c r="H62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2012,6 +2200,9 @@
         <v>12</v>
       </c>
       <c r="G63" t="n">
+        <v>7</v>
+      </c>
+      <c r="H63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2037,6 +2228,9 @@
         <v>50</v>
       </c>
       <c r="G64" t="n">
+        <v>21</v>
+      </c>
+      <c r="H64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2062,6 +2256,9 @@
         <v>39</v>
       </c>
       <c r="G65" t="n">
+        <v>15</v>
+      </c>
+      <c r="H65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2087,6 +2284,9 @@
         <v>36</v>
       </c>
       <c r="G66" t="n">
+        <v>9</v>
+      </c>
+      <c r="H66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2112,6 +2312,9 @@
         <v>26</v>
       </c>
       <c r="G67" t="n">
+        <v>4</v>
+      </c>
+      <c r="H67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2137,6 +2340,9 @@
         <v>3</v>
       </c>
       <c r="G68" t="n">
+        <v>8</v>
+      </c>
+      <c r="H68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2162,6 +2368,9 @@
         <v>0</v>
       </c>
       <c r="G69" t="n">
+        <v>5</v>
+      </c>
+      <c r="H69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2187,6 +2396,9 @@
         <v>0</v>
       </c>
       <c r="G70" t="n">
+        <v>5</v>
+      </c>
+      <c r="H70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2212,6 +2424,9 @@
         <v>0</v>
       </c>
       <c r="G71" t="n">
+        <v>3</v>
+      </c>
+      <c r="H71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2237,6 +2452,9 @@
         <v>0</v>
       </c>
       <c r="G72" t="n">
+        <v>3</v>
+      </c>
+      <c r="H72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2262,6 +2480,9 @@
         <v>0</v>
       </c>
       <c r="G73" t="n">
+        <v>10</v>
+      </c>
+      <c r="H73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2287,6 +2508,9 @@
         <v>6</v>
       </c>
       <c r="G74" t="n">
+        <v>14</v>
+      </c>
+      <c r="H74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2312,6 +2536,9 @@
         <v>10</v>
       </c>
       <c r="G75" t="n">
+        <v>19</v>
+      </c>
+      <c r="H75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2337,6 +2564,9 @@
         <v>15</v>
       </c>
       <c r="G76" t="n">
+        <v>18</v>
+      </c>
+      <c r="H76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2362,6 +2592,9 @@
         <v>49</v>
       </c>
       <c r="G77" t="n">
+        <v>27</v>
+      </c>
+      <c r="H77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2387,6 +2620,9 @@
         <v>44</v>
       </c>
       <c r="G78" t="n">
+        <v>23</v>
+      </c>
+      <c r="H78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2412,6 +2648,9 @@
         <v>39</v>
       </c>
       <c r="G79" t="n">
+        <v>25</v>
+      </c>
+      <c r="H79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2437,6 +2676,9 @@
         <v>5</v>
       </c>
       <c r="G80" t="n">
+        <v>27</v>
+      </c>
+      <c r="H80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2462,6 +2704,9 @@
         <v>0</v>
       </c>
       <c r="G81" t="n">
+        <v>14</v>
+      </c>
+      <c r="H81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2487,6 +2732,9 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
+        <v>9</v>
+      </c>
+      <c r="H82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2512,6 +2760,9 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
+        <v>8</v>
+      </c>
+      <c r="H83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2537,6 +2788,9 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
+        <v>6</v>
+      </c>
+      <c r="H84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2562,6 +2816,9 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
+        <v>9</v>
+      </c>
+      <c r="H85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2587,6 +2844,9 @@
         <v>23</v>
       </c>
       <c r="G86" t="n">
+        <v>15</v>
+      </c>
+      <c r="H86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2612,6 +2872,9 @@
         <v>4</v>
       </c>
       <c r="G87" t="n">
+        <v>12</v>
+      </c>
+      <c r="H87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2637,6 +2900,9 @@
         <v>0</v>
       </c>
       <c r="G88" t="n">
+        <v>7</v>
+      </c>
+      <c r="H88" t="n">
         <v>18.651428571</v>
       </c>
     </row>
@@ -2662,6 +2928,9 @@
         <v>0</v>
       </c>
       <c r="G89" t="n">
+        <v>7</v>
+      </c>
+      <c r="H89" t="n">
         <v>43.98</v>
       </c>
     </row>
@@ -2687,6 +2956,9 @@
         <v>23</v>
       </c>
       <c r="G90" t="n">
+        <v>9</v>
+      </c>
+      <c r="H90" t="n">
         <v>45.568571429</v>
       </c>
     </row>
@@ -2712,6 +2984,9 @@
         <v>26</v>
       </c>
       <c r="G91" t="n">
+        <v>4</v>
+      </c>
+      <c r="H91" t="n">
         <v>83.528571429</v>
       </c>
     </row>
@@ -2737,6 +3012,9 @@
         <v>31</v>
       </c>
       <c r="G92" t="n">
+        <v>18</v>
+      </c>
+      <c r="H92" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2762,6 +3040,9 @@
         <v>15</v>
       </c>
       <c r="G93" t="n">
+        <v>16</v>
+      </c>
+      <c r="H93" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2787,6 +3068,9 @@
         <v>7</v>
       </c>
       <c r="G94" t="n">
+        <v>11</v>
+      </c>
+      <c r="H94" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2812,6 +3096,9 @@
         <v>0</v>
       </c>
       <c r="G95" t="n">
+        <v>10</v>
+      </c>
+      <c r="H95" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2837,6 +3124,9 @@
         <v>0</v>
       </c>
       <c r="G96" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="H96" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2862,6 +3152,9 @@
         <v>0</v>
       </c>
       <c r="G97" t="n">
+        <v>11</v>
+      </c>
+      <c r="H97" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2887,6 +3180,9 @@
         <v>0</v>
       </c>
       <c r="G98" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="H98" t="n">
         <v>87.95999999999999</v>
       </c>
     </row>
@@ -2912,6 +3208,9 @@
         <v>0</v>
       </c>
       <c r="G99" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="H99" t="n">
         <v>76.84999999999999</v>
       </c>
     </row>
@@ -2937,6 +3236,9 @@
         <v>0</v>
       </c>
       <c r="G100" t="n">
+        <v>8</v>
+      </c>
+      <c r="H100" t="n">
         <v>76.84999999999999</v>
       </c>
     </row>
@@ -2962,6 +3264,9 @@
         <v>32</v>
       </c>
       <c r="G101" t="n">
+        <v>5</v>
+      </c>
+      <c r="H101" t="n">
         <v>75.264285714</v>
       </c>
     </row>
@@ -2987,6 +3292,9 @@
         <v>38</v>
       </c>
       <c r="G102" t="n">
+        <v>6</v>
+      </c>
+      <c r="H102" t="n">
         <v>72.617142857</v>
       </c>
     </row>
@@ -3012,6 +3320,9 @@
         <v>9</v>
       </c>
       <c r="G103" t="n">
+        <v>5</v>
+      </c>
+      <c r="H103" t="n">
         <v>72.22</v>
       </c>
     </row>
@@ -3037,6 +3348,9 @@
         <v>2</v>
       </c>
       <c r="G104" t="n">
+        <v>9</v>
+      </c>
+      <c r="H104" t="n">
         <v>72.22</v>
       </c>
     </row>
@@ -3062,6 +3376,9 @@
         <v>18</v>
       </c>
       <c r="G105" t="n">
+        <v>8</v>
+      </c>
+      <c r="H105" t="n">
         <v>51.85</v>
       </c>
     </row>
@@ -3087,6 +3404,9 @@
         <v>6</v>
       </c>
       <c r="G106" t="n">
+        <v>4</v>
+      </c>
+      <c r="H106" t="n">
         <v>51.85</v>
       </c>
     </row>
@@ -3112,6 +3432,9 @@
         <v>0</v>
       </c>
       <c r="G107" t="n">
+        <v>6</v>
+      </c>
+      <c r="H107" t="n">
         <v>50.264285714</v>
       </c>
     </row>
@@ -3137,6 +3460,9 @@
         <v>0</v>
       </c>
       <c r="G108" t="n">
+        <v>6</v>
+      </c>
+      <c r="H108" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -3162,6 +3488,9 @@
         <v>0</v>
       </c>
       <c r="G109" t="n">
+        <v>4</v>
+      </c>
+      <c r="H109" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -3187,6 +3516,9 @@
         <v>1</v>
       </c>
       <c r="G110" t="n">
+        <v>3</v>
+      </c>
+      <c r="H110" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -3212,6 +3544,9 @@
         <v>5</v>
       </c>
       <c r="G111" t="n">
+        <v>3</v>
+      </c>
+      <c r="H111" t="n">
         <v>46.3</v>
       </c>
     </row>
@@ -3237,6 +3572,9 @@
         <v>2</v>
       </c>
       <c r="G112" t="n">
+        <v>3</v>
+      </c>
+      <c r="H112" t="n">
         <v>47.092857143</v>
       </c>
     </row>
@@ -3262,6 +3600,9 @@
         <v>0</v>
       </c>
       <c r="G113" t="n">
+        <v>4</v>
+      </c>
+      <c r="H113" t="n">
         <v>48.15</v>
       </c>
     </row>
@@ -3287,6 +3628,9 @@
         <v>0</v>
       </c>
       <c r="G114" t="n">
+        <v>4</v>
+      </c>
+      <c r="H114" t="n">
         <v>48.15</v>
       </c>
     </row>
@@ -3312,6 +3656,9 @@
         <v>9</v>
       </c>
       <c r="G115" t="n">
+        <v>5</v>
+      </c>
+      <c r="H115" t="n">
         <v>48.015714286</v>
       </c>
     </row>
@@ -3337,6 +3684,9 @@
         <v>53</v>
       </c>
       <c r="G116" t="n">
+        <v>8</v>
+      </c>
+      <c r="H116" t="n">
         <v>48.61</v>
       </c>
     </row>
@@ -3362,6 +3712,9 @@
         <v>16</v>
       </c>
       <c r="G117" t="n">
+        <v>7</v>
+      </c>
+      <c r="H117" t="n">
         <v>48.61</v>
       </c>
     </row>
@@ -3387,6 +3740,9 @@
         <v>44</v>
       </c>
       <c r="G118" t="n">
+        <v>8</v>
+      </c>
+      <c r="H118" t="n">
         <v>47.818571429</v>
       </c>
     </row>
@@ -3412,6 +3768,9 @@
         <v>43</v>
       </c>
       <c r="G119" t="n">
+        <v>9</v>
+      </c>
+      <c r="H119" t="n">
         <v>49.54</v>
       </c>
     </row>
@@ -3437,6 +3796,9 @@
         <v>34</v>
       </c>
       <c r="G120" t="n">
+        <v>6</v>
+      </c>
+      <c r="H120" t="n">
         <v>47.951428571</v>
       </c>
     </row>
@@ -3462,6 +3824,9 @@
         <v>4</v>
       </c>
       <c r="G121" t="n">
+        <v>11</v>
+      </c>
+      <c r="H121" t="n">
         <v>45.568571429</v>
       </c>
     </row>
@@ -3487,6 +3852,9 @@
         <v>0</v>
       </c>
       <c r="G122" t="n">
+        <v>9</v>
+      </c>
+      <c r="H122" t="n">
         <v>49.54</v>
       </c>
     </row>
@@ -3512,6 +3880,9 @@
         <v>1</v>
       </c>
       <c r="G123" t="n">
+        <v>7</v>
+      </c>
+      <c r="H123" t="n">
         <v>62.037142857</v>
       </c>
     </row>
@@ -3537,6 +3908,9 @@
         <v>1</v>
       </c>
       <c r="G124" t="n">
+        <v>5</v>
+      </c>
+      <c r="H124" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -3562,6 +3936,9 @@
         <v>1</v>
       </c>
       <c r="G125" t="n">
+        <v>7</v>
+      </c>
+      <c r="H125" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -3587,6 +3964,9 @@
         <v>4</v>
       </c>
       <c r="G126" t="n">
+        <v>10</v>
+      </c>
+      <c r="H126" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -3612,6 +3992,9 @@
         <v>6</v>
       </c>
       <c r="G127" t="n">
+        <v>18</v>
+      </c>
+      <c r="H127" t="n">
         <v>77.642857143</v>
       </c>
     </row>
@@ -3637,6 +4020,9 @@
         <v>17</v>
       </c>
       <c r="G128" t="n">
+        <v>34</v>
+      </c>
+      <c r="H128" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3662,6 +4048,9 @@
         <v>59</v>
       </c>
       <c r="G129" t="n">
+        <v>27</v>
+      </c>
+      <c r="H129" t="n">
         <v>75</v>
       </c>
     </row>
@@ -3687,6 +4076,9 @@
         <v>88</v>
       </c>
       <c r="G130" t="n">
+        <v>36</v>
+      </c>
+      <c r="H130" t="n">
         <v>65.477142857</v>
       </c>
     </row>
@@ -3712,6 +4104,9 @@
         <v>82</v>
       </c>
       <c r="G131" t="n">
+        <v>60</v>
+      </c>
+      <c r="H131" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3737,6 +4132,9 @@
         <v>39</v>
       </c>
       <c r="G132" t="n">
+        <v>54</v>
+      </c>
+      <c r="H132" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3762,6 +4160,9 @@
         <v>0</v>
       </c>
       <c r="G133" t="n">
+        <v>15</v>
+      </c>
+      <c r="H133" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3787,6 +4188,9 @@
         <v>0</v>
       </c>
       <c r="G134" t="n">
+        <v>16</v>
+      </c>
+      <c r="H134" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3812,6 +4216,9 @@
         <v>0</v>
       </c>
       <c r="G135" t="n">
+        <v>17</v>
+      </c>
+      <c r="H135" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3837,6 +4244,9 @@
         <v>0</v>
       </c>
       <c r="G136" t="n">
+        <v>10</v>
+      </c>
+      <c r="H136" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3862,6 +4272,9 @@
         <v>1</v>
       </c>
       <c r="G137" t="n">
+        <v>9</v>
+      </c>
+      <c r="H137" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -3887,6 +4300,9 @@
         <v>21</v>
       </c>
       <c r="G138" t="n">
+        <v>18</v>
+      </c>
+      <c r="H138" t="n">
         <v>60.19</v>
       </c>
     </row>
@@ -3912,6 +4328,9 @@
         <v>2</v>
       </c>
       <c r="G139" t="n">
+        <v>14</v>
+      </c>
+      <c r="H139" t="n">
         <v>60.19</v>
       </c>
     </row>
@@ -3937,6 +4356,9 @@
         <v>0</v>
       </c>
       <c r="G140" t="n">
+        <v>11</v>
+      </c>
+      <c r="H140" t="n">
         <v>64.552857143</v>
       </c>
     </row>
@@ -3962,6 +4384,9 @@
         <v>0</v>
       </c>
       <c r="G141" t="n">
+        <v>9</v>
+      </c>
+      <c r="H141" t="n">
         <v>66.00714285700001</v>
       </c>
     </row>
@@ -3987,6 +4412,9 @@
         <v>16</v>
       </c>
       <c r="G142" t="n">
+        <v>13</v>
+      </c>
+      <c r="H142" t="n">
         <v>65.61</v>
       </c>
     </row>
@@ -4012,6 +4440,9 @@
         <v>11</v>
       </c>
       <c r="G143" t="n">
+        <v>8</v>
+      </c>
+      <c r="H143" t="n">
         <v>65.61</v>
       </c>
     </row>
@@ -4037,6 +4468,9 @@
         <v>34</v>
       </c>
       <c r="G144" t="n">
+        <v>17</v>
+      </c>
+      <c r="H144" t="n">
         <v>69.577142857</v>
       </c>
     </row>
@@ -4062,6 +4496,9 @@
         <v>42</v>
       </c>
       <c r="G145" t="n">
+        <v>22</v>
+      </c>
+      <c r="H145" t="n">
         <v>68.52</v>
       </c>
     </row>
@@ -4087,6 +4524,9 @@
         <v>36</v>
       </c>
       <c r="G146" t="n">
+        <v>11</v>
+      </c>
+      <c r="H146" t="n">
         <v>74.471428571</v>
       </c>
     </row>
@@ -4112,6 +4552,9 @@
         <v>27</v>
       </c>
       <c r="G147" t="n">
+        <v>9</v>
+      </c>
+      <c r="H147" t="n">
         <v>75</v>
       </c>
     </row>
@@ -4137,6 +4580,9 @@
         <v>45</v>
       </c>
       <c r="G148" t="n">
+        <v>6</v>
+      </c>
+      <c r="H148" t="n">
         <v>75</v>
       </c>
     </row>
@@ -4162,6 +4608,9 @@
         <v>39</v>
       </c>
       <c r="G149" t="n">
+        <v>7</v>
+      </c>
+      <c r="H149" t="n">
         <v>75</v>
       </c>
     </row>
@@ -4187,6 +4636,9 @@
         <v>19</v>
       </c>
       <c r="G150" t="n">
+        <v>13</v>
+      </c>
+      <c r="H150" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -4212,6 +4664,9 @@
         <v>3</v>
       </c>
       <c r="G151" t="n">
+        <v>11</v>
+      </c>
+      <c r="H151" t="n">
         <v>63.89</v>
       </c>
     </row>
@@ -4237,6 +4692,9 @@
         <v>11</v>
       </c>
       <c r="G152" t="n">
+        <v>12</v>
+      </c>
+      <c r="H152" t="n">
         <v>57.275714286</v>
       </c>
     </row>
@@ -4262,6 +4720,9 @@
         <v>42</v>
       </c>
       <c r="G153" t="n">
+        <v>12</v>
+      </c>
+      <c r="H153" t="n">
         <v>54.63</v>
       </c>
     </row>
@@ -4287,6 +4748,9 @@
         <v>37</v>
       </c>
       <c r="G154" t="n">
+        <v>9</v>
+      </c>
+      <c r="H154" t="n">
         <v>54.63</v>
       </c>
     </row>
@@ -4312,6 +4776,9 @@
         <v>9</v>
       </c>
       <c r="G155" t="n">
+        <v>10</v>
+      </c>
+      <c r="H155" t="n">
         <v>54.63</v>
       </c>
     </row>
@@ -4337,6 +4804,9 @@
         <v>3</v>
       </c>
       <c r="G156" t="n">
+        <v>9</v>
+      </c>
+      <c r="H156" t="n">
         <v>53.571428571</v>
       </c>
     </row>
@@ -4362,6 +4832,9 @@
         <v>2</v>
       </c>
       <c r="G157" t="n">
+        <v>5</v>
+      </c>
+      <c r="H157" t="n">
         <v>47.22</v>
       </c>
     </row>
@@ -4387,6 +4860,9 @@
         <v>2</v>
       </c>
       <c r="G158" t="n">
+        <v>7</v>
+      </c>
+      <c r="H158" t="n">
         <v>46.227142857</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created and tested Off trade visibility
</commit_message>
<xml_diff>
--- a/OUTPUT_DF/control_df.xlsx
+++ b/OUTPUT_DF/control_df.xlsx
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.004034727766019211</v>
+        <v>0.004042878238050786</v>
       </c>
       <c r="E2" t="n">
         <v>0.1666666666666667</v>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-0.003652486835248147</v>
+        <v>-0.003645824618894783</v>
       </c>
       <c r="E3" t="n">
         <v>0.1666666666666667</v>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-0.006235258055066545</v>
+        <v>-0.006215859173511962</v>
       </c>
       <c r="E5" t="n">
         <v>0.1666666666666667</v>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-0.00968659940641187</v>
+        <v>-0.009639835418859662</v>
       </c>
       <c r="E6" t="n">
         <v>0.1666666666666667</v>
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.01395029322421881</v>
+        <v>0.01404805262655181</v>
       </c>
       <c r="E7" t="n">
         <v>0.1666666666666667</v>
@@ -651,7 +651,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.01254757352393429</v>
+        <v>0.01262662461170637</v>
       </c>
       <c r="E8" t="n">
         <v>0.1666666666666667</v>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.00450013546274506</v>
+        <v>0.004510276278311522</v>
       </c>
       <c r="E9" t="n">
         <v>0.1666666666666667</v>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.008829448487061124</v>
+        <v>0.008868543043768587</v>
       </c>
       <c r="E10" t="n">
         <v>0.1666666666666667</v>
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.03521333901604005</v>
+        <v>0.03584067045832369</v>
       </c>
       <c r="E11" t="n">
         <v>0.1666666666666667</v>
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.02950060593747095</v>
+        <v>0.02994005955097757</v>
       </c>
       <c r="E12" t="n">
         <v>0.1666666666666667</v>
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.03681799175613665</v>
+        <v>0.03750416934055106</v>
       </c>
       <c r="E13" t="n">
         <v>0.1666666666666667</v>
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.04447319895146391</v>
+        <v>0.04547695645631788</v>
       </c>
       <c r="E14" t="n">
         <v>0.1666666666666667</v>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.05358513318660785</v>
+        <v>0.05504680744112762</v>
       </c>
       <c r="E15" t="n">
         <v>0.1547619047619048</v>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.04259081657257695</v>
+        <v>0.04351082014668525</v>
       </c>
       <c r="E16" t="n">
         <v>0.1666666666666667</v>
@@ -903,7 +903,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.02198908082029977</v>
+        <v>0.02223262246779819</v>
       </c>
       <c r="E17" t="n">
         <v>0.1547619047619048</v>
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.01130355643973088</v>
+        <v>0.01136768302554992</v>
       </c>
       <c r="E18" t="n">
         <v>0.1666666666666667</v>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.01556871373029011</v>
+        <v>0.01569053754619044</v>
       </c>
       <c r="E19" t="n">
         <v>0.1666666666666667</v>
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.02555939954859926</v>
+        <v>0.02588884179477095</v>
       </c>
       <c r="E20" t="n">
         <v>0.1547619047619048</v>
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.008027154973763795</v>
+        <v>0.008059458960769459</v>
       </c>
       <c r="E21" t="n">
         <v>0.1547619047619048</v>
@@ -1043,7 +1043,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.01867961453903383</v>
+        <v>0.01885516993741128</v>
       </c>
       <c r="E22" t="n">
         <v>0.1547619047619048</v>
@@ -1071,7 +1071,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.05760112085918486</v>
+        <v>0.05929238179483087</v>
       </c>
       <c r="E23" t="n">
         <v>0.1666666666666667</v>
@@ -1099,7 +1099,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.07484688568677077</v>
+        <v>0.07771912402743743</v>
       </c>
       <c r="E24" t="n">
         <v>0.1666666666666667</v>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.04626323537411289</v>
+        <v>0.04735007426180416</v>
       </c>
       <c r="E25" t="n">
         <v>0.1785714285714286</v>
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.05437264215409243</v>
+        <v>0.05587799350338602</v>
       </c>
       <c r="E26" t="n">
         <v>0.1785714285714286</v>
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.05064101736794163</v>
+        <v>0.05194519543873719</v>
       </c>
       <c r="E27" t="n">
         <v>0.1785714285714286</v>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.01818067777897367</v>
+        <v>0.01834695243469221</v>
       </c>
       <c r="E28" t="n">
         <v>0.1785714285714286</v>
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.01388979310241541</v>
+        <v>0.01398670445165816</v>
       </c>
       <c r="E29" t="n">
         <v>0.1785714285714286</v>
@@ -1267,7 +1267,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.01367927032789854</v>
+        <v>0.01377325962560057</v>
       </c>
       <c r="E30" t="n">
         <v>0.1785714285714286</v>
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.01456377378651633</v>
+        <v>0.01467034225785346</v>
       </c>
       <c r="E31" t="n">
         <v>0.1666666666666667</v>
@@ -1323,7 +1323,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.003047253383390853</v>
+        <v>0.003051900979584161</v>
       </c>
       <c r="E32" t="n">
         <v>0.1547619047619048</v>
@@ -1351,7 +1351,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.01867474951167743</v>
+        <v>0.01885021319119481</v>
       </c>
       <c r="E33" t="n">
         <v>0.1547619047619048</v>
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.004045152543858919</v>
+        <v>0.004053345216555855</v>
       </c>
       <c r="E34" t="n">
         <v>0.1547619047619048</v>
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.01843410564893042</v>
+        <v>0.01860506263850282</v>
       </c>
       <c r="E35" t="n">
         <v>0.1547619047619048</v>
@@ -1435,7 +1435,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.01579117601220473</v>
+        <v>0.0159165155157475</v>
       </c>
       <c r="E36" t="n">
         <v>0.1547619047619048</v>
@@ -1463,7 +1463,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.02271937350701201</v>
+        <v>0.02297942413481227</v>
       </c>
       <c r="E37" t="n">
         <v>0.1547619047619048</v>
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.01962757215821579</v>
+        <v>0.01982145938695859</v>
       </c>
       <c r="E38" t="n">
         <v>0.1547619047619048</v>
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.01937221827473221</v>
+        <v>0.01956107726305238</v>
       </c>
       <c r="E39" t="n">
         <v>0.1547619047619048</v>
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.03248660847614245</v>
+        <v>0.03302005933857501</v>
       </c>
       <c r="E40" t="n">
         <v>0.1547619047619048</v>
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.03516925559223718</v>
+        <v>0.03579500806154041</v>
       </c>
       <c r="E41" t="n">
         <v>0.1666666666666667</v>
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.03309894677845424</v>
+        <v>0.03365281079717002</v>
       </c>
       <c r="E42" t="n">
         <v>0.1547619047619048</v>
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.0285169492581372</v>
+        <v>0.02892745024368969</v>
       </c>
       <c r="E43" t="n">
         <v>0.1547619047619048</v>
@@ -1659,7 +1659,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.01070836387313437</v>
+        <v>0.01076590360360181</v>
       </c>
       <c r="E44" t="n">
         <v>0.1547619047619048</v>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.007875574967370414</v>
+        <v>0.007906668881788287</v>
       </c>
       <c r="E45" t="n">
         <v>0.1547619047619048</v>
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>-0.002289178648226958</v>
+        <v>-0.002286560476986865</v>
       </c>
       <c r="E46" t="n">
         <v>0.1547619047619048</v>
@@ -1743,7 +1743,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.01522342873919984</v>
+        <v>0.01533989538720435</v>
       </c>
       <c r="E47" t="n">
         <v>0.1547619047619048</v>
@@ -1771,7 +1771,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.01850686253593583</v>
+        <v>0.01867917586803967</v>
       </c>
       <c r="E48" t="n">
         <v>0.1547619047619048</v>
@@ -1799,7 +1799,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.01111170385397318</v>
+        <v>0.01117366813213433</v>
       </c>
       <c r="E49" t="n">
         <v>0.1547619047619048</v>
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.01002225445216644</v>
+        <v>0.010072645447418</v>
       </c>
       <c r="E50" t="n">
         <v>0.1547619047619048</v>
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.01137675501299126</v>
+        <v>0.01144171640652512</v>
       </c>
       <c r="E51" t="n">
         <v>0.1547619047619048</v>
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.007347829316574565</v>
+        <v>0.007374890854990709</v>
       </c>
       <c r="E52" t="n">
         <v>0.1547619047619048</v>
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.004434293954786269</v>
+        <v>0.004444139984241941</v>
       </c>
       <c r="E53" t="n">
         <v>0.1547619047619048</v>
@@ -1939,7 +1939,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.004733245539153396</v>
+        <v>0.004744465040387339</v>
       </c>
       <c r="E54" t="n">
         <v>0.1547619047619048</v>
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.00278185777810078</v>
+        <v>0.00278573073495533</v>
       </c>
       <c r="E55" t="n">
         <v>0.1547619047619048</v>
@@ -1995,7 +1995,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.007268932406056768</v>
+        <v>0.007295415223601011</v>
       </c>
       <c r="E56" t="n">
         <v>0.1547619047619048</v>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.0005635901970911153</v>
+        <v>0.0005637490438862749</v>
       </c>
       <c r="E57" t="n">
         <v>0.1428571428571428</v>
@@ -2051,7 +2051,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.001360767750296443</v>
+        <v>0.001361694014827555</v>
       </c>
       <c r="E58" t="n">
         <v>0.1428571428571428</v>
@@ -2079,7 +2079,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.006579608802793816</v>
+        <v>0.006601301980234997</v>
       </c>
       <c r="E59" t="n">
         <v>0.1428571428571428</v>
@@ -2107,7 +2107,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.009583862130579197</v>
+        <v>0.009629934403060036</v>
       </c>
       <c r="E60" t="n">
         <v>0.1428571428571428</v>
@@ -2135,7 +2135,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.003561744653356064</v>
+        <v>0.003568095203284521</v>
       </c>
       <c r="E61" t="n">
         <v>0.130952380952381</v>
@@ -2163,7 +2163,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.005540539488117736</v>
+        <v>0.00555591666319215</v>
       </c>
       <c r="E62" t="n">
         <v>0.119047619047619</v>
@@ -2191,7 +2191,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.01743319897094744</v>
+        <v>0.01758604408539041</v>
       </c>
       <c r="E63" t="n">
         <v>0.130952380952381</v>
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.008164500434874924</v>
+        <v>0.008197920860326854</v>
       </c>
       <c r="E64" t="n">
         <v>0.130952380952381</v>
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.01073016343231211</v>
+        <v>0.01078793809490256</v>
       </c>
       <c r="E65" t="n">
         <v>0.130952380952381</v>
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.0169149173029911</v>
+        <v>0.01705878453945363</v>
       </c>
       <c r="E66" t="n">
         <v>0.1428571428571428</v>
@@ -2303,7 +2303,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.01663740438499015</v>
+        <v>0.01677657674834243</v>
       </c>
       <c r="E67" t="n">
         <v>0.09523809523809523</v>
@@ -2331,7 +2331,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.01256307036933456</v>
+        <v>0.01264231725154905</v>
       </c>
       <c r="E68" t="n">
         <v>0.09523809523809523</v>
@@ -2359,7 +2359,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.004903710417211724</v>
+        <v>0.00491575328200014</v>
       </c>
       <c r="E69" t="n">
         <v>0.09523809523809523</v>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.0001242889194008451</v>
+        <v>0.000124296643588534</v>
       </c>
       <c r="E70" t="n">
         <v>0.09523809523809523</v>
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>-0.002335413003600234</v>
+        <v>-0.002332688048362988</v>
       </c>
       <c r="E71" t="n">
         <v>0.09523809523809523</v>
@@ -2443,7 +2443,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.009262530228667635</v>
+        <v>0.00930556021469009</v>
       </c>
       <c r="E72" t="n">
         <v>0.09523809523809523</v>
@@ -2471,7 +2471,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.0008106444775059619</v>
+        <v>0.0008109731385434648</v>
       </c>
       <c r="E73" t="n">
         <v>0.1071428571428571</v>
@@ -2499,7 +2499,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.01058680715270364</v>
+        <v>0.0106430456824909</v>
       </c>
       <c r="E74" t="n">
         <v>0.09523809523809523</v>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.01569481807676036</v>
+        <v>0.01581862861389407</v>
       </c>
       <c r="E75" t="n">
         <v>0.1071428571428571</v>
@@ -2555,7 +2555,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.03681704102737446</v>
+        <v>0.03750318295596523</v>
       </c>
       <c r="E76" t="n">
         <v>0.09523809523809523</v>
@@ -2583,7 +2583,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.05231892312623063</v>
+        <v>0.05371174197441392</v>
       </c>
       <c r="E77" t="n">
         <v>0.119047619047619</v>
@@ -2611,7 +2611,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.04026561908612234</v>
+        <v>0.0410872701187275</v>
       </c>
       <c r="E78" t="n">
         <v>0.130952380952381</v>
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.03194262104914274</v>
+        <v>0.03245826223359115</v>
       </c>
       <c r="E79" t="n">
         <v>0.1428571428571428</v>
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.002828196590327276</v>
+        <v>0.002832199711285557</v>
       </c>
       <c r="E80" t="n">
         <v>0.130952380952381</v>
@@ -2695,7 +2695,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.005642551149875327</v>
+        <v>0.005658500325517286</v>
       </c>
       <c r="E81" t="n">
         <v>0.130952380952381</v>
@@ -2723,7 +2723,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.00965565121936794</v>
+        <v>0.009702417417778489</v>
       </c>
       <c r="E82" t="n">
         <v>0.119047619047619</v>
@@ -2751,7 +2751,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.004912892396111082</v>
+        <v>0.004924980439604139</v>
       </c>
       <c r="E83" t="n">
         <v>0.08333333333333333</v>
@@ -2779,7 +2779,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.0005888132455438922</v>
+        <v>0.000588986630091703</v>
       </c>
       <c r="E84" t="n">
         <v>0.03571428571428571</v>
@@ -2807,7 +2807,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>-0.004260287744343218</v>
+        <v>-0.004251225592203683</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
@@ -2835,7 +2835,7 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.001189007667551305</v>
+        <v>0.001189714817409103</v>
       </c>
       <c r="E86" t="n">
         <v>0.08333333333333333</v>
@@ -2863,7 +2863,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.006939172453089029</v>
+        <v>0.006963304296303718</v>
       </c>
       <c r="E87" t="n">
         <v>0.08333333333333333</v>
@@ -2891,7 +2891,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>-3.107464370894401e-05</v>
+        <v>-3.107416089722819e-05</v>
       </c>
       <c r="E88" t="n">
         <v>0.08333333333333333</v>
@@ -2919,7 +2919,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>-0.002731570822729588</v>
+        <v>-0.002727843477757794</v>
       </c>
       <c r="E89" t="n">
         <v>0.07142857142857142</v>
@@ -2947,7 +2947,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.008991972697265985</v>
+        <v>0.009032521931835831</v>
       </c>
       <c r="E90" t="n">
         <v>0.07142857142857142</v>
@@ -2975,7 +2975,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>-0.008152364194303978</v>
+        <v>-0.008119223792017195</v>
       </c>
       <c r="E91" t="n">
         <v>0.04761904761904762</v>
@@ -3003,7 +3003,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.002584094415187901</v>
+        <v>0.002587436064920819</v>
       </c>
       <c r="E92" t="n">
         <v>0.04761904761904762</v>
@@ -3031,7 +3031,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.002476541124255196</v>
+        <v>0.002479610285336932</v>
       </c>
       <c r="E93" t="n">
         <v>0.02380952380952381</v>
@@ -3059,7 +3059,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.002943781648588592</v>
+        <v>0.002948118828645366</v>
       </c>
       <c r="E94" t="n">
         <v>0.02380952380952381</v>
@@ -3087,7 +3087,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>-0.01900442560897979</v>
+        <v>-0.01882498006378161</v>
       </c>
       <c r="E95" t="n">
         <v>0.03571428571428571</v>
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>-0.01562154577015635</v>
+        <v>-0.01550016231174452</v>
       </c>
       <c r="E96" t="n">
         <v>0.03571428571428571</v>
@@ -3143,7 +3143,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>-0.02023764422383352</v>
+        <v>-0.0200342375701069</v>
       </c>
       <c r="E97" t="n">
         <v>0.02380952380952381</v>
@@ -3171,7 +3171,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>-0.0155398519556115</v>
+        <v>-0.01541973147927897</v>
       </c>
       <c r="E98" t="n">
         <v>0.04761904761904762</v>
@@ -3199,7 +3199,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>-0.004986784762649699</v>
+        <v>-0.004974371394352546</v>
       </c>
       <c r="E99" t="n">
         <v>0.07142857142857142</v>
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.0002354810938828598</v>
+        <v>0.0002355088217320197</v>
       </c>
       <c r="E100" t="n">
         <v>0.08333333333333333</v>
@@ -3255,7 +3255,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0.008746980757410669</v>
+        <v>0.008785347376034038</v>
       </c>
       <c r="E101" t="n">
         <v>0.08333333333333333</v>
@@ -3283,7 +3283,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0.003100039220989352</v>
+        <v>0.003104849311780922</v>
       </c>
       <c r="E102" t="n">
         <v>0.1071428571428571</v>
@@ -3311,7 +3311,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0.000480468173680484</v>
+        <v>0.000480583617001574</v>
       </c>
       <c r="E103" t="n">
         <v>0.119047619047619</v>
@@ -3339,7 +3339,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0.00538699032764811</v>
+        <v>0.00540152624994577</v>
       </c>
       <c r="E104" t="n">
         <v>0.119047619047619</v>
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0.01433111688781056</v>
+        <v>0.01443429966234874</v>
       </c>
       <c r="E105" t="n">
         <v>0.119047619047619</v>
@@ -3395,7 +3395,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0.009777546357939915</v>
+        <v>0.009825502735464554</v>
       </c>
       <c r="E106" t="n">
         <v>0.119047619047619</v>
@@ -3423,7 +3423,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0.008296424136416784</v>
+        <v>0.008330934835588565</v>
       </c>
       <c r="E107" t="n">
         <v>0.130952380952381</v>
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0.004779554082304271</v>
+        <v>0.004790994370146754</v>
       </c>
       <c r="E108" t="n">
         <v>0.130952380952381</v>
@@ -3479,7 +3479,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0.01022652029850562</v>
+        <v>0.01027898986504554</v>
       </c>
       <c r="E109" t="n">
         <v>0.130952380952381</v>
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0.01147196410410921</v>
+        <v>0.0115380194374522</v>
       </c>
       <c r="E110" t="n">
         <v>0.130952380952381</v>
@@ -3535,7 +3535,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0.01495171420750315</v>
+        <v>0.01506405026027822</v>
       </c>
       <c r="E111" t="n">
         <v>0.130952380952381</v>
@@ -3563,7 +3563,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0.0176738758334347</v>
+        <v>0.01783098297617112</v>
       </c>
       <c r="E112" t="n">
         <v>0.130952380952381</v>
@@ -3591,7 +3591,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0.01241238820614243</v>
+        <v>0.01248974161214816</v>
       </c>
       <c r="E113" t="n">
         <v>0.130952380952381</v>
@@ -3619,7 +3619,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>0.01829190865080234</v>
+        <v>0.0184602303539197</v>
       </c>
       <c r="E114" t="n">
         <v>0.119047619047619</v>
@@ -3647,7 +3647,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0.02271122930368995</v>
+        <v>0.02297109281631392</v>
       </c>
       <c r="E115" t="n">
         <v>0.130952380952381</v>
@@ -3675,7 +3675,7 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>0.02483060736198625</v>
+        <v>0.02514145440066442</v>
       </c>
       <c r="E116" t="n">
         <v>0.1547619047619048</v>
@@ -3703,7 +3703,7 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>0.03025426912248452</v>
+        <v>0.0307165800373274</v>
       </c>
       <c r="E117" t="n">
         <v>0.1428571428571428</v>
@@ -3731,7 +3731,7 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0.05413258065632754</v>
+        <v>0.0556245482732465</v>
       </c>
       <c r="E118" t="n">
         <v>0.1428571428571428</v>
@@ -3759,7 +3759,7 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0.04843081824170002</v>
+        <v>0.04962275456074702</v>
       </c>
       <c r="E119" t="n">
         <v>0.119047619047619</v>
@@ -3787,7 +3787,7 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0.04135594063929158</v>
+        <v>0.04222300905587501</v>
       </c>
       <c r="E120" t="n">
         <v>0.130952380952381</v>
@@ -3815,7 +3815,7 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>0.02115944543274189</v>
+        <v>0.02138489381135306</v>
       </c>
       <c r="E121" t="n">
         <v>0.1428571428571428</v>
@@ -3843,7 +3843,7 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0.01508423014601739</v>
+        <v>0.015198571338447</v>
       </c>
       <c r="E122" t="n">
         <v>0.1428571428571428</v>
@@ -3871,7 +3871,7 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0.00443738911121695</v>
+        <v>0.004447248900792334</v>
       </c>
       <c r="E123" t="n">
         <v>0.130952380952381</v>
@@ -3899,7 +3899,7 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>-0.002663539907622035</v>
+        <v>-0.002659995832495723</v>
       </c>
       <c r="E124" t="n">
         <v>0.130952380952381</v>
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0.001827423728256047</v>
+        <v>0.001829094484568897</v>
       </c>
       <c r="E125" t="n">
         <v>0.119047619047619</v>
@@ -3955,7 +3955,7 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>0.003647451381532653</v>
+        <v>0.003654111427258842</v>
       </c>
       <c r="E126" t="n">
         <v>0.130952380952381</v>
@@ -3983,7 +3983,7 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0.01814484409510526</v>
+        <v>0.01831046196572818</v>
       </c>
       <c r="E127" t="n">
         <v>0.130952380952381</v>
@@ -4011,7 +4011,7 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>0.04219486836176774</v>
+        <v>0.04309772569188999</v>
       </c>
       <c r="E128" t="n">
         <v>0.1547619047619048</v>
@@ -4039,7 +4039,7 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>0.06597945623659511</v>
+        <v>0.0682047719944721</v>
       </c>
       <c r="E129" t="n">
         <v>0.1666666666666667</v>
@@ -4067,7 +4067,7 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>0.0480313805725991</v>
+        <v>0.04920357941697441</v>
       </c>
       <c r="E130" t="n">
         <v>0.1785714285714286</v>
@@ -4095,7 +4095,7 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>0.03262586036263665</v>
+        <v>0.03316391934678064</v>
       </c>
       <c r="E131" t="n">
         <v>0.1785714285714286</v>
@@ -4123,7 +4123,7 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>0.02491272382368888</v>
+        <v>0.02522563884606168</v>
       </c>
       <c r="E132" t="n">
         <v>0.1785714285714286</v>
@@ -4151,7 +4151,7 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>0.01182863617724419</v>
+        <v>0.01189887114893825</v>
       </c>
       <c r="E133" t="n">
         <v>0.1785714285714286</v>
@@ -4179,7 +4179,7 @@
         </is>
       </c>
       <c r="D134" t="n">
-        <v>0.01245684324353774</v>
+        <v>0.01253475288195534</v>
       </c>
       <c r="E134" t="n">
         <v>0.1785714285714286</v>
@@ -4207,7 +4207,7 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0.0148783859449537</v>
+        <v>0.01498962010604645</v>
       </c>
       <c r="E135" t="n">
         <v>0.1666666666666667</v>
@@ -4235,7 +4235,7 @@
         </is>
       </c>
       <c r="D136" t="n">
-        <v>0.01376802809051519</v>
+        <v>0.01386324386526648</v>
       </c>
       <c r="E136" t="n">
         <v>0.1547619047619048</v>
@@ -4263,7 +4263,7 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>0.01444338249507196</v>
+        <v>0.01454819213801149</v>
       </c>
       <c r="E137" t="n">
         <v>0.1547619047619048</v>
@@ -4291,7 +4291,7 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0.01389728731213731</v>
+        <v>0.01399430350915098</v>
       </c>
       <c r="E138" t="n">
         <v>0.1666666666666667</v>
@@ -4319,7 +4319,7 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>0.01502864744202661</v>
+        <v>0.01514214542493136</v>
       </c>
       <c r="E139" t="n">
         <v>0.1666666666666667</v>
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0.01563125726841101</v>
+        <v>0.01575406441262136</v>
       </c>
       <c r="E140" t="n">
         <v>0.1666666666666667</v>
@@ -4375,7 +4375,7 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0.018015076877317</v>
+        <v>0.01817832722379854</v>
       </c>
       <c r="E141" t="n">
         <v>0.1666666666666667</v>
@@ -4403,7 +4403,7 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>0.02581236773749168</v>
+        <v>0.02614839186465605</v>
       </c>
       <c r="E142" t="n">
         <v>0.1666666666666667</v>
@@ -4431,7 +4431,7 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>0.0230118592788356</v>
+        <v>0.02327867482239076</v>
       </c>
       <c r="E143" t="n">
         <v>0.1547619047619048</v>
@@ -4459,7 +4459,7 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>0.01594786518951187</v>
+        <v>0.01607571111056404</v>
       </c>
       <c r="E144" t="n">
         <v>0.1547619047619048</v>
@@ -4487,7 +4487,7 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>0.02809851251502965</v>
+        <v>0.02849699925705078</v>
       </c>
       <c r="E145" t="n">
         <v>0.1666666666666667</v>
@@ -4515,7 +4515,7 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>0.001800671236309095</v>
+        <v>0.001802293418285858</v>
       </c>
       <c r="E146" t="n">
         <v>0.1666666666666667</v>
@@ -4543,7 +4543,7 @@
         </is>
       </c>
       <c r="D147" t="n">
-        <v>-0.0004506748932470333</v>
+        <v>-0.0004505733545715613</v>
       </c>
       <c r="E147" t="n">
         <v>0.1666666666666667</v>
@@ -4571,7 +4571,7 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0.01737311568163392</v>
+        <v>0.01752490600540901</v>
       </c>
       <c r="E148" t="n">
         <v>0.1666666666666667</v>
@@ -4599,7 +4599,7 @@
         </is>
       </c>
       <c r="D149" t="n">
-        <v>0.01200811627223967</v>
+        <v>0.01208050315363511</v>
       </c>
       <c r="E149" t="n">
         <v>0.1666666666666667</v>
@@ -4627,7 +4627,7 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>0.003474428050545215</v>
+        <v>0.003480470872107215</v>
       </c>
       <c r="E150" t="n">
         <v>0.1666666666666667</v>
@@ -4655,7 +4655,7 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>-0.002051826131524507</v>
+        <v>-0.002049722575244058</v>
       </c>
       <c r="E151" t="n">
         <v>0.1666666666666667</v>
@@ -4683,7 +4683,7 @@
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0.007689060222708656</v>
+        <v>0.007718696957111732</v>
       </c>
       <c r="E152" t="n">
         <v>0.1666666666666667</v>
@@ -4711,7 +4711,7 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>0.01210186438738531</v>
+        <v>0.01217538824076082</v>
       </c>
       <c r="E153" t="n">
         <v>0.1666666666666667</v>
@@ -4739,7 +4739,7 @@
         </is>
       </c>
       <c r="D154" t="n">
-        <v>0.009578065752443458</v>
+        <v>0.009624082223143824</v>
       </c>
       <c r="E154" t="n">
         <v>0.1666666666666667</v>
@@ -4767,7 +4767,7 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>0.006131251934973499</v>
+        <v>0.006150086533666155</v>
       </c>
       <c r="E155" t="n">
         <v>0.1666666666666667</v>
@@ -4795,7 +4795,7 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0.01149321151501131</v>
+        <v>0.01155951222972661</v>
       </c>
       <c r="E156" t="n">
         <v>0.1666666666666667</v>
@@ -4823,7 +4823,7 @@
         </is>
       </c>
       <c r="D157" t="n">
-        <v>0.00267705192264671</v>
+        <v>0.002680638425849306</v>
       </c>
       <c r="E157" t="n">
         <v>0.1666666666666667</v>
@@ -4851,7 +4851,7 @@
         </is>
       </c>
       <c r="D158" t="n">
-        <v>0.005879027449751367</v>
+        <v>0.005896342847564461</v>
       </c>
       <c r="E158" t="n">
         <v>0.1547619047619048</v>

</xml_diff>

<commit_message>
changed data prep pipeline
</commit_message>
<xml_diff>
--- a/OUTPUT_DF/control_df.xlsx
+++ b/OUTPUT_DF/control_df.xlsx
@@ -479,20 +479,20 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.004042878238050786</v>
+        <v>-0.000755070638773578</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G2" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -507,20 +507,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-0.003645824618894783</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -535,20 +535,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-0.0023005887912552</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -563,20 +563,20 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-0.006215859173511962</v>
+        <v>0.003101670918833577</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F5" t="n">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G5" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -591,20 +591,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-0.009639835418859662</v>
+        <v>0.004697797155616752</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F6" t="n">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="G6" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -619,20 +619,20 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.01404805262655181</v>
+        <v>0.002378957185222189</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="G7" t="n">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -647,20 +647,20 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.01262662461170637</v>
+        <v>0.002117303653251161</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="G8" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -675,20 +675,20 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.004510276278311522</v>
+        <v>0.002101627672492546</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="G9" t="n">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -703,20 +703,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.008868543043768587</v>
+        <v>0.006172880431713447</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G10" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -731,20 +731,20 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.03584067045832369</v>
+        <v>0.004154394517860536</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F11" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G11" t="n">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -759,20 +759,20 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.02994005955097757</v>
+        <v>0.002481396826364468</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F12" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G12" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -787,20 +787,20 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.03750416934055106</v>
+        <v>0.002464672994755865</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F13" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="G13" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -815,20 +815,20 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.04547695645631788</v>
+        <v>0.03543366013260521</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F14" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G14" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -843,20 +843,20 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.05504680744112762</v>
+        <v>0.04150349288691185</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F15" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G15" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -871,20 +871,20 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.04351082014668525</v>
+        <v>0.03256393064014376</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F16" t="n">
         <v>29</v>
       </c>
       <c r="G16" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -899,20 +899,20 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.02223262246779819</v>
+        <v>0.01397933308998778</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="G17" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -927,20 +927,20 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.01136768302554992</v>
+        <v>0.01386305176373523</v>
       </c>
       <c r="E18" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F18" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G18" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -955,20 +955,20 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.01569053754619044</v>
+        <v>0.003110094580476946</v>
       </c>
       <c r="E19" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G19" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -983,20 +983,20 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.02588884179477095</v>
+        <v>0.02272422121994667</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G20" t="n">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1011,20 +1011,20 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.008059458960769459</v>
+        <v>0.00352083912584532</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F21" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G21" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1039,20 +1039,20 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.01885516993741128</v>
+        <v>0.01215320447149034</v>
       </c>
       <c r="E22" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F22" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G22" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1067,20 +1067,20 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.05929238179483087</v>
+        <v>0.007937631396755214</v>
       </c>
       <c r="E23" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F23" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="G23" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1095,20 +1095,20 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.07771912402743743</v>
+        <v>0.01698608418270394</v>
       </c>
       <c r="E24" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F24" t="n">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G24" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1123,20 +1123,20 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.04735007426180416</v>
+        <v>0.01308072829589028</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F25" t="n">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="G25" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1151,20 +1151,20 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.05587799350338602</v>
+        <v>0.01510769907042788</v>
       </c>
       <c r="E26" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F26" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G26" t="n">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
@@ -1179,20 +1179,20 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.05194519543873719</v>
+        <v>0.01222410353511274</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F27" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G27" t="n">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -1207,20 +1207,20 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.01834695243469221</v>
+        <v>0.003414730187523015</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G28" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1235,20 +1235,20 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.01398670445165816</v>
+        <v>0.03726962823471006</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G29" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1263,20 +1263,20 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.01377325962560057</v>
+        <v>0.01253512658108402</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G30" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1291,20 +1291,20 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.01467034225785346</v>
+        <v>0.003637748489022921</v>
       </c>
       <c r="E31" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1319,20 +1319,20 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.003051900979584161</v>
+        <v>-0.01485425883056215</v>
       </c>
       <c r="E32" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G32" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1347,20 +1347,20 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.01885021319119481</v>
+        <v>0.02288468778394557</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F33" t="n">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="G33" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1375,20 +1375,20 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.004053345216555855</v>
+        <v>0.01148581168291831</v>
       </c>
       <c r="E34" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F34" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G34" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -1403,20 +1403,20 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.01860506263850282</v>
+        <v>0.01033465832326398</v>
       </c>
       <c r="E35" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F35" t="n">
         <v>8</v>
       </c>
       <c r="G35" t="n">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -1431,20 +1431,20 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.0159165155157475</v>
+        <v>0.01041982759822606</v>
       </c>
       <c r="E36" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F36" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1459,20 +1459,20 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.02297942413481227</v>
+        <v>0.01491878149848453</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G37" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
@@ -1487,20 +1487,20 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.01982145938695859</v>
+        <v>0.01043451825257207</v>
       </c>
       <c r="E38" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F38" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G38" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H38" t="n">
         <v>0</v>
@@ -1515,17 +1515,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.01956107726305238</v>
+        <v>0.007023504440674107</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1547619047619048</v>
+        <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="G39" t="n">
         <v>15</v>
@@ -1543,20 +1543,20 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.03302005933857501</v>
+        <v>0.007820833146087103</v>
       </c>
       <c r="E40" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F40" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G40" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -1571,20 +1571,20 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.03579500806154041</v>
+        <v>0.008690585191936122</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F41" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -1599,20 +1599,20 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.03365281079717002</v>
+        <v>0.01055448488542959</v>
       </c>
       <c r="E42" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F42" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="G42" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -1627,20 +1627,20 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.02892745024368969</v>
+        <v>0.01206092087226486</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F43" t="n">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G43" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -1655,20 +1655,20 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.01076590360360181</v>
+        <v>0.009691637397433317</v>
       </c>
       <c r="E44" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -1683,20 +1683,20 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.007906668881788287</v>
+        <v>0.01089774698983685</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G45" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H45" t="n">
         <v>0</v>
@@ -1711,20 +1711,20 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>-0.002286560476986865</v>
+        <v>0.009684005781253682</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F46" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G46" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -1739,20 +1739,20 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.01533989538720435</v>
+        <v>0.004505032532613161</v>
       </c>
       <c r="E47" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F47" t="n">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="G47" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -1767,20 +1767,20 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0.01867917586803967</v>
+        <v>0.009789435764383091</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F48" t="n">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G48" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -1795,20 +1795,20 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.01117366813213433</v>
+        <v>0.007896089336321582</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F49" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G49" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -1823,20 +1823,20 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.010072645447418</v>
+        <v>0.04463257588880598</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F50" t="n">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="G50" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -1851,20 +1851,20 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.01144171640652512</v>
+        <v>0.007825310557779599</v>
       </c>
       <c r="E51" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F51" t="n">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="G51" t="n">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -1879,20 +1879,20 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0.007374890854990709</v>
+        <v>0.005830171586509581</v>
       </c>
       <c r="E52" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F52" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G52" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
@@ -1907,20 +1907,20 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0.004444139984241941</v>
+        <v>0.00437113444692316</v>
       </c>
       <c r="E53" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="G53" t="n">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
@@ -1935,20 +1935,20 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.004744465040387339</v>
+        <v>0.002545820485515261</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F54" t="n">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="G54" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="H54" t="n">
         <v>0</v>
@@ -1963,20 +1963,20 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.00278573073495533</v>
+        <v>0.003197490231616198</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F55" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="G55" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
@@ -1991,20 +1991,20 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0.007295415223601011</v>
+        <v>0.005302044169953019</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F56" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="G56" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2019,20 +2019,20 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.0005637490438862749</v>
+        <v>0.005704508042787212</v>
       </c>
       <c r="E57" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G57" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
@@ -2047,20 +2047,20 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0.001361694014827555</v>
+        <v>0.009090172517134055</v>
       </c>
       <c r="E58" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="G58" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
@@ -2075,20 +2075,20 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.006601301980234997</v>
+        <v>0.007606325146227353</v>
       </c>
       <c r="E59" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F59" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="G59" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H59" t="n">
         <v>0</v>
@@ -2103,20 +2103,20 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.009629934403060036</v>
+        <v>0.007307142415619871</v>
       </c>
       <c r="E60" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F60" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="G60" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="H60" t="n">
         <v>0</v>
@@ -2131,20 +2131,20 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>0.003568095203284521</v>
+        <v>0.006653400945457578</v>
       </c>
       <c r="E61" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="G61" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -2159,20 +2159,20 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0.00555591666319215</v>
+        <v>0.007690430348873847</v>
       </c>
       <c r="E62" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F62" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G62" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
@@ -2187,20 +2187,20 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0.01758604408539041</v>
+        <v>0.006448453933323168</v>
       </c>
       <c r="E63" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F63" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G63" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
@@ -2215,20 +2215,20 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.008197920860326854</v>
+        <v>0.008200075498693608</v>
       </c>
       <c r="E64" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F64" t="n">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="G64" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H64" t="n">
         <v>0</v>
@@ -2243,20 +2243,20 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0.01078793809490256</v>
+        <v>0.01178235339397138</v>
       </c>
       <c r="E65" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F65" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G65" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H65" t="n">
         <v>0</v>
@@ -2271,20 +2271,20 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.01705878453945363</v>
+        <v>0.02844714076958525</v>
       </c>
       <c r="E66" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F66" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G66" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H66" t="n">
         <v>0</v>
@@ -2299,20 +2299,20 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.01677657674834243</v>
+        <v>0.01080954111593122</v>
       </c>
       <c r="E67" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F67" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G67" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="H67" t="n">
         <v>0</v>
@@ -2327,20 +2327,20 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.01264231725154905</v>
+        <v>0.007825440334571283</v>
       </c>
       <c r="E68" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F68" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G68" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="H68" t="n">
         <v>0</v>
@@ -2355,20 +2355,20 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.00491575328200014</v>
+        <v>0.01378572695054878</v>
       </c>
       <c r="E69" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="G69" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -2383,20 +2383,20 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.000124296643588534</v>
+        <v>0.02715259814087369</v>
       </c>
       <c r="E70" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="G70" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="H70" t="n">
         <v>0</v>
@@ -2411,20 +2411,20 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>-0.002332688048362988</v>
+        <v>0.03569393226003413</v>
       </c>
       <c r="E71" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G71" t="n">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
@@ -2439,20 +2439,20 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.00930556021469009</v>
+        <v>0.03088047603857828</v>
       </c>
       <c r="E72" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G72" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="H72" t="n">
         <v>0</v>
@@ -2467,20 +2467,20 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0.0008109731385434648</v>
+        <v>0.02579766790691434</v>
       </c>
       <c r="E73" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G73" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="H73" t="n">
         <v>0</v>
@@ -2495,20 +2495,20 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0.0106430456824909</v>
+        <v>0.0105822329735973</v>
       </c>
       <c r="E74" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F74" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="G74" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="H74" t="n">
         <v>0</v>
@@ -2523,20 +2523,20 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.01581862861389407</v>
+        <v>0.01790255139203105</v>
       </c>
       <c r="E75" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F75" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G75" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H75" t="n">
         <v>0</v>
@@ -2551,20 +2551,20 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.03750318295596523</v>
+        <v>0.01386153067190398</v>
       </c>
       <c r="E76" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F76" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G76" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H76" t="n">
         <v>0</v>
@@ -2579,20 +2579,20 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.05371174197441392</v>
+        <v>0.01400517204100869</v>
       </c>
       <c r="E77" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F77" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G77" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H77" t="n">
         <v>0</v>
@@ -2607,20 +2607,20 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.0410872701187275</v>
+        <v>0.0143223944506718</v>
       </c>
       <c r="E78" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F78" t="n">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="G78" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H78" t="n">
         <v>0</v>
@@ -2635,20 +2635,20 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.03245826223359115</v>
+        <v>0.01179564814916764</v>
       </c>
       <c r="E79" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F79" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G79" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H79" t="n">
         <v>0</v>
@@ -2663,20 +2663,20 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0.002832199711285557</v>
+        <v>0.006542962425941732</v>
       </c>
       <c r="E80" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F80" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G80" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -2691,20 +2691,20 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.005658500325517286</v>
+        <v>0.03464152064965953</v>
       </c>
       <c r="E81" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="G81" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H81" t="n">
         <v>0</v>
@@ -2719,20 +2719,20 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.009702417417778489</v>
+        <v>0.02264941868386761</v>
       </c>
       <c r="E82" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G82" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H82" t="n">
         <v>0</v>
@@ -2747,20 +2747,20 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0.004924980439604139</v>
+        <v>0.008371128671742719</v>
       </c>
       <c r="E83" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G83" t="n">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="H83" t="n">
         <v>0</v>
@@ -2775,20 +2775,20 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.000588986630091703</v>
+        <v>0.006269717046145053</v>
       </c>
       <c r="E84" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F84" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G84" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="H84" t="n">
         <v>0</v>
@@ -2803,20 +2803,20 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>-0.004251225592203683</v>
+        <v>0.00318567247486958</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G85" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H85" t="n">
         <v>0</v>
@@ -2831,20 +2831,20 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0.001189714817409103</v>
+        <v>0.0002767931389714694</v>
       </c>
       <c r="E86" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F86" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G86" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H86" t="n">
         <v>0</v>
@@ -2859,20 +2859,20 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.006963304296303718</v>
+        <v>-0.0002869853509251468</v>
       </c>
       <c r="E87" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F87" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H87" t="n">
         <v>0</v>
@@ -2887,20 +2887,20 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>-3.107416089722819e-05</v>
+        <v>-0.0002720456314996333</v>
       </c>
       <c r="E88" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
       </c>
       <c r="G88" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="H88" t="n">
         <v>18.651428571</v>
@@ -2915,20 +2915,20 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>-0.002727843477757794</v>
+        <v>0.003571348907385504</v>
       </c>
       <c r="E89" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G89" t="n">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="H89" t="n">
         <v>43.98</v>
@@ -2943,20 +2943,20 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.009032521931835831</v>
+        <v>0.002331480227889832</v>
       </c>
       <c r="E90" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F90" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G90" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="H90" t="n">
         <v>45.568571429</v>
@@ -2971,20 +2971,20 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>-0.008119223792017195</v>
+        <v>-3.527607193329877e-05</v>
       </c>
       <c r="E91" t="n">
-        <v>0.04761904761904762</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F91" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="G91" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="H91" t="n">
         <v>83.528571429</v>
@@ -2999,20 +2999,20 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.002587436064920819</v>
+        <v>-0.0005569389141133346</v>
       </c>
       <c r="E92" t="n">
-        <v>0.04761904761904762</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F92" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="G92" t="n">
-        <v>18</v>
+        <v>20.5</v>
       </c>
       <c r="H92" t="n">
         <v>87.95999999999999</v>
@@ -3027,20 +3027,20 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0.002479610285336932</v>
+        <v>0.003639806497956753</v>
       </c>
       <c r="E93" t="n">
-        <v>0.02380952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F93" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G93" t="n">
-        <v>16</v>
+        <v>23.5</v>
       </c>
       <c r="H93" t="n">
         <v>87.95999999999999</v>
@@ -3055,20 +3055,20 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.002948118828645366</v>
+        <v>0.004696267324961371</v>
       </c>
       <c r="E94" t="n">
-        <v>0.02380952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F94" t="n">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="G94" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H94" t="n">
         <v>87.95999999999999</v>
@@ -3083,20 +3083,20 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>-0.01882498006378161</v>
+        <v>0.002267929313189486</v>
       </c>
       <c r="E95" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F95" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G95" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H95" t="n">
         <v>87.95999999999999</v>
@@ -3111,20 +3111,20 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>-0.01550016231174452</v>
+        <v>0.001299394348995923</v>
       </c>
       <c r="E96" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G96" t="n">
-        <v>10.5</v>
+        <v>22.5</v>
       </c>
       <c r="H96" t="n">
         <v>87.95999999999999</v>
@@ -3139,20 +3139,20 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>-0.0200342375701069</v>
+        <v>0.00212934198648457</v>
       </c>
       <c r="E97" t="n">
-        <v>0.02380952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F97" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G97" t="n">
-        <v>11</v>
+        <v>25.5</v>
       </c>
       <c r="H97" t="n">
         <v>87.95999999999999</v>
@@ -3167,20 +3167,20 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>-0.01541973147927897</v>
+        <v>0.001377083796975972</v>
       </c>
       <c r="E98" t="n">
-        <v>0.04761904761904762</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F98" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G98" t="n">
-        <v>10.5</v>
+        <v>26.5</v>
       </c>
       <c r="H98" t="n">
         <v>87.95999999999999</v>
@@ -3195,20 +3195,20 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>-0.004974371394352546</v>
+        <v>0.002981657044506518</v>
       </c>
       <c r="E99" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F99" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G99" t="n">
-        <v>9.5</v>
+        <v>22</v>
       </c>
       <c r="H99" t="n">
         <v>76.84999999999999</v>
@@ -3223,20 +3223,20 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.0002355088217320197</v>
+        <v>0.001890622948251248</v>
       </c>
       <c r="E100" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F100" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G100" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H100" t="n">
         <v>76.84999999999999</v>
@@ -3251,20 +3251,20 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0.008785347376034038</v>
+        <v>-6.482993427956871e-05</v>
       </c>
       <c r="E101" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F101" t="n">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G101" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H101" t="n">
         <v>75.264285714</v>
@@ -3279,20 +3279,20 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0.003104849311780922</v>
+        <v>0.03743306260835856</v>
       </c>
       <c r="E102" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F102" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G102" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H102" t="n">
         <v>72.617142857</v>
@@ -3307,20 +3307,20 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0.000480583617001574</v>
+        <v>0.005197993886685044</v>
       </c>
       <c r="E103" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F103" t="n">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G103" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="H103" t="n">
         <v>72.22</v>
@@ -3335,20 +3335,20 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0.00540152624994577</v>
+        <v>0.001983272616301942</v>
       </c>
       <c r="E104" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F104" t="n">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="G104" t="n">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="H104" t="n">
         <v>72.22</v>
@@ -3363,20 +3363,20 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>0.01443429966234874</v>
+        <v>0.0001411042877328555</v>
       </c>
       <c r="E105" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F105" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G105" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H105" t="n">
         <v>51.85</v>
@@ -3391,20 +3391,20 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0.009825502735464554</v>
+        <v>0.0002904243942506539</v>
       </c>
       <c r="E106" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F106" t="n">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="G106" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="H106" t="n">
         <v>51.85</v>
@@ -3419,20 +3419,20 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0.008330934835588565</v>
+        <v>-0.0008273607067611426</v>
       </c>
       <c r="E107" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F107" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G107" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="H107" t="n">
         <v>50.264285714</v>
@@ -3447,20 +3447,20 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0.004790994370146754</v>
+        <v>-0.001414245312102238</v>
       </c>
       <c r="E108" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F108" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G108" t="n">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="H108" t="n">
         <v>46.3</v>
@@ -3475,20 +3475,20 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0.01027898986504554</v>
+        <v>-0.0007213864818561709</v>
       </c>
       <c r="E109" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F109" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G109" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="H109" t="n">
         <v>46.3</v>
@@ -3503,20 +3503,20 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0.0115380194374522</v>
+        <v>0.004376896017556402</v>
       </c>
       <c r="E110" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F110" t="n">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="G110" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="H110" t="n">
         <v>46.3</v>
@@ -3531,20 +3531,20 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0.01506405026027822</v>
+        <v>0.002639431139571133</v>
       </c>
       <c r="E111" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F111" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="G111" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="H111" t="n">
         <v>46.3</v>
@@ -3559,20 +3559,20 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>0.01783098297617112</v>
+        <v>0.0007634974224028804</v>
       </c>
       <c r="E112" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F112" t="n">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="G112" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="H112" t="n">
         <v>47.092857143</v>
@@ -3587,20 +3587,20 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0.01248974161214816</v>
+        <v>0.002503560850889579</v>
       </c>
       <c r="E113" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F113" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G113" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H113" t="n">
         <v>48.15</v>
@@ -3615,20 +3615,20 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>0.0184602303539197</v>
+        <v>0.005358659026915535</v>
       </c>
       <c r="E114" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F114" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G114" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="H114" t="n">
         <v>48.15</v>
@@ -3643,20 +3643,20 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0.02297109281631392</v>
+        <v>0.002284018263936385</v>
       </c>
       <c r="E115" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F115" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G115" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="H115" t="n">
         <v>48.015714286</v>
@@ -3671,20 +3671,20 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>0.02514145440066442</v>
+        <v>0.00240019628538921</v>
       </c>
       <c r="E116" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F116" t="n">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="G116" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H116" t="n">
         <v>48.61</v>
@@ -3699,20 +3699,20 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>0.0307165800373274</v>
+        <v>0.02004738767318043</v>
       </c>
       <c r="E117" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F117" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="G117" t="n">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="H117" t="n">
         <v>48.61</v>
@@ -3727,20 +3727,20 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0.0556245482732465</v>
+        <v>0.02484160924992753</v>
       </c>
       <c r="E118" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F118" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G118" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H118" t="n">
         <v>47.818571429</v>
@@ -3755,20 +3755,20 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0.04962275456074702</v>
+        <v>0.006341762531922348</v>
       </c>
       <c r="E119" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F119" t="n">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="G119" t="n">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="H119" t="n">
         <v>49.54</v>
@@ -3783,20 +3783,20 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0.04222300905587501</v>
+        <v>0.004039360578522472</v>
       </c>
       <c r="E120" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F120" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="G120" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H120" t="n">
         <v>47.951428571</v>
@@ -3811,20 +3811,20 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>0.02138489381135306</v>
+        <v>0.003742992946637556</v>
       </c>
       <c r="E121" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F121" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G121" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H121" t="n">
         <v>45.568571429</v>
@@ -3839,20 +3839,20 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0.015198571338447</v>
+        <v>0.008440493188665873</v>
       </c>
       <c r="E122" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F122" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G122" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="H122" t="n">
         <v>49.54</v>
@@ -3867,20 +3867,20 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0.004447248900792334</v>
+        <v>0.01991904741416087</v>
       </c>
       <c r="E123" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F123" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G123" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H123" t="n">
         <v>62.037142857</v>
@@ -3895,20 +3895,20 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>-0.002659995832495723</v>
+        <v>0.02572893309590481</v>
       </c>
       <c r="E124" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F124" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="G124" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="H124" t="n">
         <v>78.7</v>
@@ -3923,20 +3923,20 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0.001829094484568897</v>
+        <v>0.01992083323778775</v>
       </c>
       <c r="E125" t="n">
-        <v>0.119047619047619</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F125" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G125" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="H125" t="n">
         <v>78.7</v>
@@ -3951,20 +3951,20 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>0.003654111427258842</v>
+        <v>0.005286479339530283</v>
       </c>
       <c r="E126" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F126" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="G126" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H126" t="n">
         <v>78.7</v>
@@ -3979,20 +3979,20 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0.01831046196572818</v>
+        <v>0.005556197629816253</v>
       </c>
       <c r="E127" t="n">
-        <v>0.130952380952381</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F127" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="G127" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H127" t="n">
         <v>77.642857143</v>
@@ -4007,20 +4007,20 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>0.04309772569188999</v>
+        <v>0.01233426019797245</v>
       </c>
       <c r="E128" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F128" t="n">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="G128" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H128" t="n">
         <v>75</v>
@@ -4035,20 +4035,20 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>0.0682047719944721</v>
+        <v>0.008415870828738934</v>
       </c>
       <c r="E129" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F129" t="n">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="G129" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H129" t="n">
         <v>75</v>
@@ -4063,20 +4063,20 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>0.04920357941697441</v>
+        <v>0.009680382819717856</v>
       </c>
       <c r="E130" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F130" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="G130" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H130" t="n">
         <v>65.477142857</v>
@@ -4091,20 +4091,20 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>0.03316391934678064</v>
+        <v>0.01147904732748661</v>
       </c>
       <c r="E131" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F131" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G131" t="n">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="H131" t="n">
         <v>63.89</v>
@@ -4119,20 +4119,20 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>0.02522563884606168</v>
+        <v>0.006436357158480325</v>
       </c>
       <c r="E132" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F132" t="n">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="G132" t="n">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="H132" t="n">
         <v>63.89</v>
@@ -4147,20 +4147,20 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>0.01189887114893825</v>
+        <v>0.005210144203667675</v>
       </c>
       <c r="E133" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F133" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G133" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H133" t="n">
         <v>63.89</v>
@@ -4175,20 +4175,20 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>0.01253475288195534</v>
+        <v>0.03332145399187561</v>
       </c>
       <c r="E134" t="n">
-        <v>0.1785714285714286</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F134" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G134" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H134" t="n">
         <v>63.89</v>
@@ -4203,20 +4203,20 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0.01498962010604645</v>
+        <v>0.01947487679103742</v>
       </c>
       <c r="E135" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F135" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G135" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H135" t="n">
         <v>63.89</v>
@@ -4231,20 +4231,20 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>0.01386324386526648</v>
+        <v>0.004663629770938988</v>
       </c>
       <c r="E136" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F136" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G136" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H136" t="n">
         <v>63.89</v>
@@ -4259,20 +4259,20 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>0.01454819213801149</v>
+        <v>0.0005189010792343414</v>
       </c>
       <c r="E137" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F137" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="G137" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="H137" t="n">
         <v>63.89</v>
@@ -4287,20 +4287,20 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0.01399430350915098</v>
+        <v>0.02013964665953423</v>
       </c>
       <c r="E138" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F138" t="n">
+        <v>13</v>
+      </c>
+      <c r="G138" t="n">
         <v>21</v>
-      </c>
-      <c r="G138" t="n">
-        <v>18</v>
       </c>
       <c r="H138" t="n">
         <v>60.19</v>
@@ -4315,20 +4315,20 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>0.01514214542493136</v>
+        <v>0.01461959034616894</v>
       </c>
       <c r="E139" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F139" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G139" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H139" t="n">
         <v>60.19</v>
@@ -4343,20 +4343,20 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0.01575406441262136</v>
+        <v>-0.001776756973831556</v>
       </c>
       <c r="E140" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F140" t="n">
         <v>0</v>
       </c>
       <c r="G140" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H140" t="n">
         <v>64.552857143</v>
@@ -4371,20 +4371,20 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0.01817832722379854</v>
+        <v>0.002178137166467781</v>
       </c>
       <c r="E141" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F141" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G141" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H141" t="n">
         <v>66.00714285700001</v>
@@ -4399,20 +4399,20 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>0.02614839186465605</v>
+        <v>-0.001029795664263842</v>
       </c>
       <c r="E142" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F142" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G142" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H142" t="n">
         <v>65.61</v>
@@ -4427,20 +4427,20 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>0.02327867482239076</v>
+        <v>-0.0007323480876772109</v>
       </c>
       <c r="E143" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F143" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G143" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H143" t="n">
         <v>65.61</v>
@@ -4455,20 +4455,20 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>0.01607571111056404</v>
+        <v>0.006137471391615688</v>
       </c>
       <c r="E144" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F144" t="n">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="G144" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H144" t="n">
         <v>69.577142857</v>
@@ -4483,20 +4483,20 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>0.02849699925705078</v>
+        <v>0.005941977381314426</v>
       </c>
       <c r="E145" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F145" t="n">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="G145" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H145" t="n">
         <v>68.52</v>
@@ -4511,20 +4511,20 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>0.001802293418285858</v>
+        <v>-0.00039966739306927</v>
       </c>
       <c r="E146" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F146" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="G146" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="H146" t="n">
         <v>74.471428571</v>
@@ -4539,20 +4539,20 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>-0.0004505733545715613</v>
+        <v>-0.000994432806304177</v>
       </c>
       <c r="E147" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F147" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="G147" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="H147" t="n">
         <v>75</v>
@@ -4567,20 +4567,20 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0.01752490600540901</v>
+        <v>0.00293556569940153</v>
       </c>
       <c r="E148" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F148" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G148" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H148" t="n">
         <v>75</v>
@@ -4595,20 +4595,20 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>0.01208050315363511</v>
+        <v>0.003769481709610888</v>
       </c>
       <c r="E149" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F149" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G149" t="n">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H149" t="n">
         <v>75</v>
@@ -4623,20 +4623,20 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>0.003480470872107215</v>
+        <v>0.00599894169667809</v>
       </c>
       <c r="E150" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F150" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G150" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H150" t="n">
         <v>63.89</v>
@@ -4651,20 +4651,20 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>-0.002049722575244058</v>
+        <v>0.004807201288955304</v>
       </c>
       <c r="E151" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F151" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G151" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="H151" t="n">
         <v>63.89</v>
@@ -4679,20 +4679,20 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0.007718696957111732</v>
+        <v>0.005146356503197043</v>
       </c>
       <c r="E152" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F152" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G152" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H152" t="n">
         <v>57.275714286</v>
@@ -4707,20 +4707,20 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D153" t="n">
-        <v>0.01217538824076082</v>
+        <v>0.04111699799204318</v>
       </c>
       <c r="E153" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F153" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G153" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H153" t="n">
         <v>54.63</v>
@@ -4735,20 +4735,20 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D154" t="n">
-        <v>0.009624082223143824</v>
+        <v>0.03006537557191363</v>
       </c>
       <c r="E154" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F154" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G154" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H154" t="n">
         <v>54.63</v>
@@ -4763,20 +4763,20 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>0.006150086533666155</v>
+        <v>0.004756968971478957</v>
       </c>
       <c r="E155" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F155" t="n">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G155" t="n">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H155" t="n">
         <v>54.63</v>
@@ -4791,20 +4791,20 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0.01155951222972661</v>
+        <v>0.006471816106636408</v>
       </c>
       <c r="E156" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F156" t="n">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="G156" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="H156" t="n">
         <v>53.571428571</v>
@@ -4819,20 +4819,20 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>0.002680638425849306</v>
+        <v>0.003759315811925113</v>
       </c>
       <c r="E157" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F157" t="n">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="G157" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H157" t="n">
         <v>47.22</v>
@@ -4847,20 +4847,20 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>precious_liquid</t>
+          <t>fast_duck</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>0.005896342847564461</v>
+        <v>0.001598669572276741</v>
       </c>
       <c r="E158" t="n">
-        <v>0.1547619047619048</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="F158" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G158" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="H158" t="n">
         <v>46.227142857</v>

</xml_diff>

<commit_message>
refactored data preparation pipeline
</commit_message>
<xml_diff>
--- a/OUTPUT_DF/control_df.xlsx
+++ b/OUTPUT_DF/control_df.xlsx
@@ -446,14 +446,14 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>distribution</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>promotion</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>distribution</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>epros</t>
@@ -461,12 +461,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>covid</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>off_trade_visibility</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>covid</t>
         </is>
       </c>
     </row>
@@ -483,19 +483,19 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E2" t="n">
         <v>-0.000755070638773578</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F2" t="n">
         <v>7</v>
       </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>35</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -511,19 +511,19 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0101010101010101</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0101010101010101</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
         <v>21</v>
       </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>33</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -539,19 +539,19 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E4" t="n">
         <v>-0.0023005887912552</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F4" t="n">
         <v>10</v>
       </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>30</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -567,19 +567,19 @@
         </is>
       </c>
       <c r="D5" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.003101670918833577</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F5" t="n">
         <v>44</v>
       </c>
       <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>31</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -595,19 +595,19 @@
         </is>
       </c>
       <c r="D6" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.004697797155616752</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F6" t="n">
         <v>70</v>
       </c>
       <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>32</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -623,19 +623,19 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.002378957185222189</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F7" t="n">
         <v>36</v>
       </c>
       <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>47</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -651,19 +651,19 @@
         </is>
       </c>
       <c r="D8" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.002117303653251161</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F8" t="n">
         <v>33</v>
       </c>
       <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>48</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -679,19 +679,19 @@
         </is>
       </c>
       <c r="D9" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E9" t="n">
         <v>0.002101627672492546</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F9" t="n">
         <v>31</v>
       </c>
       <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>45</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -707,19 +707,19 @@
         </is>
       </c>
       <c r="D10" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.006172880431713447</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F10" t="n">
         <v>29</v>
       </c>
       <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>33</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -735,19 +735,19 @@
         </is>
       </c>
       <c r="D11" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.004154394517860536</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F11" t="n">
         <v>28</v>
       </c>
       <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>31</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -763,19 +763,19 @@
         </is>
       </c>
       <c r="D12" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E12" t="n">
         <v>0.002481396826364468</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F12" t="n">
         <v>14</v>
       </c>
       <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>30</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -791,19 +791,19 @@
         </is>
       </c>
       <c r="D13" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.002464672994755865</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F13" t="n">
         <v>14</v>
       </c>
       <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
         <v>28</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -819,19 +819,19 @@
         </is>
       </c>
       <c r="D14" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.03543366013260521</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F14" t="n">
         <v>39</v>
       </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>25</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -847,19 +847,19 @@
         </is>
       </c>
       <c r="D15" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E15" t="n">
         <v>0.04150349288691185</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F15" t="n">
         <v>30</v>
       </c>
       <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
         <v>25</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -875,19 +875,19 @@
         </is>
       </c>
       <c r="D16" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.03256393064014376</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F16" t="n">
         <v>29</v>
       </c>
       <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
         <v>25</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -903,19 +903,19 @@
         </is>
       </c>
       <c r="D17" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.01397933308998778</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F17" t="n">
         <v>45</v>
       </c>
       <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
         <v>29</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -931,19 +931,19 @@
         </is>
       </c>
       <c r="D18" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E18" t="n">
         <v>0.01386305176373523</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F18" t="n">
         <v>35</v>
       </c>
       <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
         <v>27</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -959,19 +959,19 @@
         </is>
       </c>
       <c r="D19" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.003110094580476946</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F19" t="n">
         <v>17</v>
       </c>
       <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
         <v>32</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -987,19 +987,19 @@
         </is>
       </c>
       <c r="D20" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E20" t="n">
         <v>0.02272422121994667</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F20" t="n">
         <v>21</v>
       </c>
       <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
         <v>31</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1015,19 +1015,19 @@
         </is>
       </c>
       <c r="D21" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.00352083912584532</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F21" t="n">
         <v>10</v>
       </c>
       <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
         <v>28</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1043,19 +1043,19 @@
         </is>
       </c>
       <c r="D22" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E22" t="n">
         <v>0.01215320447149034</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F22" t="n">
         <v>24</v>
       </c>
       <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
         <v>33</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1071,19 +1071,19 @@
         </is>
       </c>
       <c r="D23" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.007937631396755214</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F23" t="n">
         <v>22</v>
       </c>
       <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
         <v>31</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1099,19 +1099,19 @@
         </is>
       </c>
       <c r="D24" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E24" t="n">
         <v>0.01698608418270394</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F24" t="n">
         <v>51</v>
       </c>
       <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
         <v>36</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1127,19 +1127,19 @@
         </is>
       </c>
       <c r="D25" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.01308072829589028</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F25" t="n">
         <v>62</v>
       </c>
       <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
         <v>24</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1155,19 +1155,19 @@
         </is>
       </c>
       <c r="D26" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E26" t="n">
         <v>0.01510769907042788</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F26" t="n">
         <v>67</v>
       </c>
       <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
         <v>39</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1183,19 +1183,19 @@
         </is>
       </c>
       <c r="D27" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E27" t="n">
         <v>0.01222410353511274</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F27" t="n">
         <v>50</v>
       </c>
       <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
         <v>37</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1211,19 +1211,19 @@
         </is>
       </c>
       <c r="D28" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E28" t="n">
         <v>0.003414730187523015</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F28" t="n">
         <v>15</v>
       </c>
       <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
         <v>34</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1239,19 +1239,19 @@
         </is>
       </c>
       <c r="D29" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E29" t="n">
         <v>0.03726962823471006</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F29" t="n">
         <v>20</v>
       </c>
       <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
         <v>30</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1267,19 +1267,19 @@
         </is>
       </c>
       <c r="D30" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E30" t="n">
         <v>0.01253512658108402</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F30" t="n">
         <v>11</v>
       </c>
       <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
         <v>23</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1295,19 +1295,19 @@
         </is>
       </c>
       <c r="D31" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E31" t="n">
         <v>0.003637748489022921</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F31" t="n">
         <v>4</v>
       </c>
       <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
         <v>24</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1323,19 +1323,19 @@
         </is>
       </c>
       <c r="D32" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E32" t="n">
         <v>-0.01485425883056215</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F32" t="n">
         <v>24</v>
       </c>
       <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
         <v>25</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1351,19 +1351,19 @@
         </is>
       </c>
       <c r="D33" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E33" t="n">
         <v>0.02288468778394557</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F33" t="n">
         <v>45</v>
       </c>
       <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
         <v>23</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1379,19 +1379,19 @@
         </is>
       </c>
       <c r="D34" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E34" t="n">
         <v>0.01148581168291831</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F34" t="n">
         <v>12</v>
       </c>
       <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
         <v>27</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1407,19 +1407,19 @@
         </is>
       </c>
       <c r="D35" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E35" t="n">
         <v>0.01033465832326398</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F35" t="n">
         <v>8</v>
       </c>
       <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
         <v>31</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1435,19 +1435,19 @@
         </is>
       </c>
       <c r="D36" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E36" t="n">
         <v>0.01041982759822606</v>
       </c>
-      <c r="E36" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
         <v>28</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1463,19 +1463,19 @@
         </is>
       </c>
       <c r="D37" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E37" t="n">
         <v>0.01491878149848453</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F37" t="n">
         <v>8</v>
       </c>
       <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
         <v>23</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1491,19 +1491,19 @@
         </is>
       </c>
       <c r="D38" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E38" t="n">
         <v>0.01043451825257207</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F38" t="n">
         <v>13</v>
       </c>
       <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
         <v>22</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1519,19 +1519,19 @@
         </is>
       </c>
       <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
         <v>0.007023504440674107</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
       </c>
       <c r="F39" t="n">
         <v>24</v>
       </c>
       <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
         <v>15</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1547,19 +1547,19 @@
         </is>
       </c>
       <c r="D40" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E40" t="n">
         <v>0.007820833146087103</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F40" t="n">
         <v>22</v>
       </c>
       <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
         <v>18</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1575,19 +1575,19 @@
         </is>
       </c>
       <c r="D41" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E41" t="n">
         <v>0.008690585191936122</v>
       </c>
-      <c r="E41" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F41" t="n">
         <v>0</v>
       </c>
       <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
         <v>22</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1603,19 +1603,19 @@
         </is>
       </c>
       <c r="D42" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E42" t="n">
         <v>0.01055448488542959</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F42" t="n">
         <v>23</v>
       </c>
       <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
         <v>21</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1631,19 +1631,19 @@
         </is>
       </c>
       <c r="D43" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E43" t="n">
         <v>0.01206092087226486</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F43" t="n">
         <v>55</v>
       </c>
       <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
         <v>22</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1659,19 +1659,19 @@
         </is>
       </c>
       <c r="D44" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E44" t="n">
         <v>0.009691637397433317</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
       </c>
       <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
         <v>24</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1687,19 +1687,19 @@
         </is>
       </c>
       <c r="D45" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E45" t="n">
         <v>0.01089774698983685</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F45" t="n">
         <v>15</v>
       </c>
       <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
         <v>26</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1715,19 +1715,19 @@
         </is>
       </c>
       <c r="D46" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E46" t="n">
         <v>0.009684005781253682</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F46" t="n">
         <v>16</v>
       </c>
       <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
         <v>26</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1743,19 +1743,19 @@
         </is>
       </c>
       <c r="D47" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E47" t="n">
         <v>0.004505032532613161</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F47" t="n">
         <v>2</v>
       </c>
       <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
         <v>22</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1771,19 +1771,19 @@
         </is>
       </c>
       <c r="D48" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E48" t="n">
         <v>0.009789435764383091</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F48" t="n">
         <v>14</v>
       </c>
       <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
         <v>22</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1799,19 +1799,19 @@
         </is>
       </c>
       <c r="D49" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E49" t="n">
         <v>0.007896089336321582</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F49" t="n">
         <v>19</v>
       </c>
       <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
         <v>25</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1827,19 +1827,19 @@
         </is>
       </c>
       <c r="D50" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E50" t="n">
         <v>0.04463257588880598</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F50" t="n">
         <v>64</v>
       </c>
       <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
         <v>22</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1855,19 +1855,19 @@
         </is>
       </c>
       <c r="D51" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E51" t="n">
         <v>0.007825310557779599</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F51" t="n">
         <v>38</v>
       </c>
       <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
         <v>27</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1883,19 +1883,19 @@
         </is>
       </c>
       <c r="D52" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E52" t="n">
         <v>0.005830171586509581</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F52" t="n">
         <v>22</v>
       </c>
       <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
         <v>33</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1911,19 +1911,19 @@
         </is>
       </c>
       <c r="D53" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E53" t="n">
         <v>0.00437113444692316</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F53" t="n">
         <v>29</v>
       </c>
       <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
         <v>29</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1939,19 +1939,19 @@
         </is>
       </c>
       <c r="D54" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E54" t="n">
         <v>0.002545820485515261</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F54" t="n">
         <v>28</v>
       </c>
       <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
         <v>29</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1967,19 +1967,19 @@
         </is>
       </c>
       <c r="D55" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E55" t="n">
         <v>0.003197490231616198</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F55" t="n">
         <v>33</v>
       </c>
       <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
         <v>27</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1995,19 +1995,19 @@
         </is>
       </c>
       <c r="D56" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E56" t="n">
         <v>0.005302044169953019</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F56" t="n">
         <v>32</v>
       </c>
       <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
         <v>29</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2023,19 +2023,19 @@
         </is>
       </c>
       <c r="D57" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E57" t="n">
         <v>0.005704508042787212</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F57" t="n">
         <v>29</v>
       </c>
       <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
         <v>34</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -2051,19 +2051,19 @@
         </is>
       </c>
       <c r="D58" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E58" t="n">
         <v>0.009090172517134055</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F58" t="n">
         <v>42</v>
       </c>
       <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
         <v>30</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2079,19 +2079,19 @@
         </is>
       </c>
       <c r="D59" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E59" t="n">
         <v>0.007606325146227353</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F59" t="n">
         <v>39</v>
       </c>
       <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
         <v>30</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2107,19 +2107,19 @@
         </is>
       </c>
       <c r="D60" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E60" t="n">
         <v>0.007307142415619871</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F60" t="n">
         <v>34</v>
       </c>
       <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
         <v>37</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2135,19 +2135,19 @@
         </is>
       </c>
       <c r="D61" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E61" t="n">
         <v>0.006653400945457578</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F61" t="n">
         <v>31</v>
       </c>
       <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
         <v>36</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2163,19 +2163,19 @@
         </is>
       </c>
       <c r="D62" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E62" t="n">
         <v>0.007690430348873847</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F62" t="n">
         <v>25</v>
       </c>
       <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
         <v>35</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2191,19 +2191,19 @@
         </is>
       </c>
       <c r="D63" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E63" t="n">
         <v>0.006448453933323168</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F63" t="n">
         <v>22</v>
       </c>
       <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
         <v>31</v>
-      </c>
-      <c r="H63" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2219,19 +2219,19 @@
         </is>
       </c>
       <c r="D64" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E64" t="n">
         <v>0.008200075498693608</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F64" t="n">
         <v>14</v>
       </c>
       <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
         <v>27</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2247,19 +2247,19 @@
         </is>
       </c>
       <c r="D65" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E65" t="n">
         <v>0.01178235339397138</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F65" t="n">
         <v>31</v>
       </c>
       <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
         <v>28</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2275,19 +2275,19 @@
         </is>
       </c>
       <c r="D66" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E66" t="n">
         <v>0.02844714076958525</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F66" t="n">
         <v>29</v>
       </c>
       <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
         <v>26</v>
-      </c>
-      <c r="H66" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2303,19 +2303,19 @@
         </is>
       </c>
       <c r="D67" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E67" t="n">
         <v>0.01080954111593122</v>
-      </c>
-      <c r="E67" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F67" t="n">
         <v>13</v>
       </c>
       <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
         <v>24</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2331,19 +2331,19 @@
         </is>
       </c>
       <c r="D68" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E68" t="n">
         <v>0.007825440334571283</v>
-      </c>
-      <c r="E68" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F68" t="n">
         <v>10</v>
       </c>
       <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
         <v>25</v>
-      </c>
-      <c r="H68" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2359,19 +2359,19 @@
         </is>
       </c>
       <c r="D69" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E69" t="n">
         <v>0.01378572695054878</v>
-      </c>
-      <c r="E69" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F69" t="n">
         <v>63</v>
       </c>
       <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
         <v>27</v>
-      </c>
-      <c r="H69" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2387,19 +2387,19 @@
         </is>
       </c>
       <c r="D70" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E70" t="n">
         <v>0.02715259814087369</v>
-      </c>
-      <c r="E70" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F70" t="n">
         <v>32</v>
       </c>
       <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
         <v>35</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2415,19 +2415,19 @@
         </is>
       </c>
       <c r="D71" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E71" t="n">
         <v>0.03569393226003413</v>
-      </c>
-      <c r="E71" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F71" t="n">
         <v>43</v>
       </c>
       <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
         <v>37</v>
-      </c>
-      <c r="H71" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2443,19 +2443,19 @@
         </is>
       </c>
       <c r="D72" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E72" t="n">
         <v>0.03088047603857828</v>
-      </c>
-      <c r="E72" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F72" t="n">
         <v>20</v>
       </c>
       <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
         <v>32</v>
-      </c>
-      <c r="H72" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2471,19 +2471,19 @@
         </is>
       </c>
       <c r="D73" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E73" t="n">
         <v>0.02579766790691434</v>
-      </c>
-      <c r="E73" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F73" t="n">
         <v>16</v>
       </c>
       <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
         <v>31</v>
-      </c>
-      <c r="H73" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2499,19 +2499,19 @@
         </is>
       </c>
       <c r="D74" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E74" t="n">
         <v>0.0105822329735973</v>
-      </c>
-      <c r="E74" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F74" t="n">
         <v>33</v>
       </c>
       <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
         <v>27</v>
-      </c>
-      <c r="H74" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2527,19 +2527,19 @@
         </is>
       </c>
       <c r="D75" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E75" t="n">
         <v>0.01790255139203105</v>
-      </c>
-      <c r="E75" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F75" t="n">
         <v>30</v>
       </c>
       <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
         <v>35</v>
-      </c>
-      <c r="H75" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2555,19 +2555,19 @@
         </is>
       </c>
       <c r="D76" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E76" t="n">
         <v>0.01386153067190398</v>
-      </c>
-      <c r="E76" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F76" t="n">
         <v>45</v>
       </c>
       <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
         <v>32</v>
-      </c>
-      <c r="H76" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2583,19 +2583,19 @@
         </is>
       </c>
       <c r="D77" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E77" t="n">
         <v>0.01400517204100869</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F77" t="n">
         <v>57</v>
       </c>
       <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="n">
         <v>26</v>
-      </c>
-      <c r="H77" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2611,19 +2611,19 @@
         </is>
       </c>
       <c r="D78" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E78" t="n">
         <v>0.0143223944506718</v>
-      </c>
-      <c r="E78" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F78" t="n">
         <v>85</v>
       </c>
       <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
         <v>25</v>
-      </c>
-      <c r="H78" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2639,19 +2639,19 @@
         </is>
       </c>
       <c r="D79" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E79" t="n">
         <v>0.01179564814916764</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F79" t="n">
         <v>24</v>
       </c>
       <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
         <v>31</v>
-      </c>
-      <c r="H79" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2667,19 +2667,19 @@
         </is>
       </c>
       <c r="D80" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E80" t="n">
         <v>0.006542962425941732</v>
-      </c>
-      <c r="E80" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F80" t="n">
         <v>9</v>
       </c>
       <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
         <v>41</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2695,19 +2695,19 @@
         </is>
       </c>
       <c r="D81" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E81" t="n">
         <v>0.03464152064965953</v>
-      </c>
-      <c r="E81" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F81" t="n">
         <v>39</v>
       </c>
       <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
         <v>26</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2723,19 +2723,19 @@
         </is>
       </c>
       <c r="D82" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E82" t="n">
         <v>0.02264941868386761</v>
-      </c>
-      <c r="E82" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F82" t="n">
         <v>34</v>
       </c>
       <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
         <v>24</v>
-      </c>
-      <c r="H82" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2751,19 +2751,19 @@
         </is>
       </c>
       <c r="D83" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E83" t="n">
         <v>0.008371128671742719</v>
-      </c>
-      <c r="E83" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F83" t="n">
         <v>22</v>
       </c>
       <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
         <v>31</v>
-      </c>
-      <c r="H83" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2779,19 +2779,19 @@
         </is>
       </c>
       <c r="D84" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E84" t="n">
         <v>0.006269717046145053</v>
-      </c>
-      <c r="E84" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F84" t="n">
         <v>23</v>
       </c>
       <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
         <v>32</v>
-      </c>
-      <c r="H84" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2807,19 +2807,19 @@
         </is>
       </c>
       <c r="D85" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E85" t="n">
         <v>0.00318567247486958</v>
-      </c>
-      <c r="E85" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F85" t="n">
         <v>13</v>
       </c>
       <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
         <v>30</v>
-      </c>
-      <c r="H85" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2835,19 +2835,19 @@
         </is>
       </c>
       <c r="D86" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E86" t="n">
         <v>0.0002767931389714694</v>
-      </c>
-      <c r="E86" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F86" t="n">
         <v>12</v>
       </c>
       <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
         <v>28</v>
-      </c>
-      <c r="H86" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2863,19 +2863,19 @@
         </is>
       </c>
       <c r="D87" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E87" t="n">
         <v>-0.0002869853509251468</v>
       </c>
-      <c r="E87" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F87" t="n">
         <v>0</v>
       </c>
       <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="n">
         <v>27</v>
-      </c>
-      <c r="H87" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2891,19 +2891,19 @@
         </is>
       </c>
       <c r="D88" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E88" t="n">
         <v>-0.0002720456314996333</v>
       </c>
-      <c r="E88" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F88" t="n">
         <v>0</v>
       </c>
       <c r="G88" t="n">
+        <v>18.651428571</v>
+      </c>
+      <c r="H88" t="n">
         <v>27</v>
-      </c>
-      <c r="H88" t="n">
-        <v>18.651428571</v>
       </c>
     </row>
     <row r="89">
@@ -2919,19 +2919,19 @@
         </is>
       </c>
       <c r="D89" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E89" t="n">
         <v>0.003571348907385504</v>
-      </c>
-      <c r="E89" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F89" t="n">
         <v>7</v>
       </c>
       <c r="G89" t="n">
+        <v>43.98</v>
+      </c>
+      <c r="H89" t="n">
         <v>28</v>
-      </c>
-      <c r="H89" t="n">
-        <v>43.98</v>
       </c>
     </row>
     <row r="90">
@@ -2947,19 +2947,19 @@
         </is>
       </c>
       <c r="D90" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E90" t="n">
         <v>0.002331480227889832</v>
-      </c>
-      <c r="E90" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F90" t="n">
         <v>11</v>
       </c>
       <c r="G90" t="n">
+        <v>45.568571429</v>
+      </c>
+      <c r="H90" t="n">
         <v>20</v>
-      </c>
-      <c r="H90" t="n">
-        <v>45.568571429</v>
       </c>
     </row>
     <row r="91">
@@ -2975,19 +2975,19 @@
         </is>
       </c>
       <c r="D91" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E91" t="n">
         <v>-3.527607193329877e-05</v>
       </c>
-      <c r="E91" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F91" t="n">
         <v>0</v>
       </c>
       <c r="G91" t="n">
+        <v>83.528571429</v>
+      </c>
+      <c r="H91" t="n">
         <v>21</v>
-      </c>
-      <c r="H91" t="n">
-        <v>83.528571429</v>
       </c>
     </row>
     <row r="92">
@@ -3003,19 +3003,19 @@
         </is>
       </c>
       <c r="D92" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E92" t="n">
         <v>-0.0005569389141133346</v>
       </c>
-      <c r="E92" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F92" t="n">
         <v>0</v>
       </c>
       <c r="G92" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H92" t="n">
         <v>20.5</v>
-      </c>
-      <c r="H92" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="93">
@@ -3031,19 +3031,19 @@
         </is>
       </c>
       <c r="D93" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E93" t="n">
         <v>0.003639806497956753</v>
-      </c>
-      <c r="E93" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F93" t="n">
         <v>33</v>
       </c>
       <c r="G93" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H93" t="n">
         <v>23.5</v>
-      </c>
-      <c r="H93" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="94">
@@ -3059,19 +3059,19 @@
         </is>
       </c>
       <c r="D94" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E94" t="n">
         <v>0.004696267324961371</v>
-      </c>
-      <c r="E94" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F94" t="n">
         <v>46</v>
       </c>
       <c r="G94" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H94" t="n">
         <v>21</v>
-      </c>
-      <c r="H94" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="95">
@@ -3087,19 +3087,19 @@
         </is>
       </c>
       <c r="D95" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E95" t="n">
         <v>0.002267929313189486</v>
-      </c>
-      <c r="E95" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F95" t="n">
         <v>5</v>
       </c>
       <c r="G95" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H95" t="n">
         <v>21</v>
-      </c>
-      <c r="H95" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="96">
@@ -3115,19 +3115,19 @@
         </is>
       </c>
       <c r="D96" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E96" t="n">
         <v>0.001299394348995923</v>
-      </c>
-      <c r="E96" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F96" t="n">
         <v>5</v>
       </c>
       <c r="G96" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H96" t="n">
         <v>22.5</v>
-      </c>
-      <c r="H96" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="97">
@@ -3143,19 +3143,19 @@
         </is>
       </c>
       <c r="D97" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E97" t="n">
         <v>0.00212934198648457</v>
-      </c>
-      <c r="E97" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F97" t="n">
         <v>37</v>
       </c>
       <c r="G97" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H97" t="n">
         <v>25.5</v>
-      </c>
-      <c r="H97" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="98">
@@ -3171,19 +3171,19 @@
         </is>
       </c>
       <c r="D98" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E98" t="n">
         <v>0.001377083796975972</v>
-      </c>
-      <c r="E98" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F98" t="n">
         <v>40</v>
       </c>
       <c r="G98" t="n">
+        <v>87.95999999999999</v>
+      </c>
+      <c r="H98" t="n">
         <v>26.5</v>
-      </c>
-      <c r="H98" t="n">
-        <v>87.95999999999999</v>
       </c>
     </row>
     <row r="99">
@@ -3199,19 +3199,19 @@
         </is>
       </c>
       <c r="D99" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E99" t="n">
         <v>0.002981657044506518</v>
-      </c>
-      <c r="E99" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F99" t="n">
         <v>16</v>
       </c>
       <c r="G99" t="n">
+        <v>76.84999999999999</v>
+      </c>
+      <c r="H99" t="n">
         <v>22</v>
-      </c>
-      <c r="H99" t="n">
-        <v>76.84999999999999</v>
       </c>
     </row>
     <row r="100">
@@ -3227,19 +3227,19 @@
         </is>
       </c>
       <c r="D100" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E100" t="n">
         <v>0.001890622948251248</v>
-      </c>
-      <c r="E100" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F100" t="n">
         <v>17</v>
       </c>
       <c r="G100" t="n">
+        <v>76.84999999999999</v>
+      </c>
+      <c r="H100" t="n">
         <v>18</v>
-      </c>
-      <c r="H100" t="n">
-        <v>76.84999999999999</v>
       </c>
     </row>
     <row r="101">
@@ -3255,19 +3255,19 @@
         </is>
       </c>
       <c r="D101" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E101" t="n">
         <v>-6.482993427956871e-05</v>
-      </c>
-      <c r="E101" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F101" t="n">
         <v>5</v>
       </c>
       <c r="G101" t="n">
+        <v>75.264285714</v>
+      </c>
+      <c r="H101" t="n">
         <v>21</v>
-      </c>
-      <c r="H101" t="n">
-        <v>75.264285714</v>
       </c>
     </row>
     <row r="102">
@@ -3283,19 +3283,19 @@
         </is>
       </c>
       <c r="D102" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E102" t="n">
         <v>0.03743306260835856</v>
-      </c>
-      <c r="E102" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F102" t="n">
         <v>44</v>
       </c>
       <c r="G102" t="n">
+        <v>72.617142857</v>
+      </c>
+      <c r="H102" t="n">
         <v>20</v>
-      </c>
-      <c r="H102" t="n">
-        <v>72.617142857</v>
       </c>
     </row>
     <row r="103">
@@ -3311,19 +3311,19 @@
         </is>
       </c>
       <c r="D103" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E103" t="n">
         <v>0.005197993886685044</v>
-      </c>
-      <c r="E103" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F103" t="n">
         <v>44</v>
       </c>
       <c r="G103" t="n">
+        <v>72.22</v>
+      </c>
+      <c r="H103" t="n">
         <v>24</v>
-      </c>
-      <c r="H103" t="n">
-        <v>72.22</v>
       </c>
     </row>
     <row r="104">
@@ -3339,19 +3339,19 @@
         </is>
       </c>
       <c r="D104" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E104" t="n">
         <v>0.001983272616301942</v>
-      </c>
-      <c r="E104" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F104" t="n">
         <v>34</v>
       </c>
       <c r="G104" t="n">
+        <v>72.22</v>
+      </c>
+      <c r="H104" t="n">
         <v>30</v>
-      </c>
-      <c r="H104" t="n">
-        <v>72.22</v>
       </c>
     </row>
     <row r="105">
@@ -3367,19 +3367,19 @@
         </is>
       </c>
       <c r="D105" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E105" t="n">
         <v>0.0001411042877328555</v>
-      </c>
-      <c r="E105" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F105" t="n">
         <v>26</v>
       </c>
       <c r="G105" t="n">
+        <v>51.85</v>
+      </c>
+      <c r="H105" t="n">
         <v>28</v>
-      </c>
-      <c r="H105" t="n">
-        <v>51.85</v>
       </c>
     </row>
     <row r="106">
@@ -3395,19 +3395,19 @@
         </is>
       </c>
       <c r="D106" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E106" t="n">
         <v>0.0002904243942506539</v>
-      </c>
-      <c r="E106" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F106" t="n">
         <v>24</v>
       </c>
       <c r="G106" t="n">
+        <v>51.85</v>
+      </c>
+      <c r="H106" t="n">
         <v>31</v>
-      </c>
-      <c r="H106" t="n">
-        <v>51.85</v>
       </c>
     </row>
     <row r="107">
@@ -3423,19 +3423,19 @@
         </is>
       </c>
       <c r="D107" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E107" t="n">
         <v>-0.0008273607067611426</v>
-      </c>
-      <c r="E107" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F107" t="n">
         <v>15</v>
       </c>
       <c r="G107" t="n">
+        <v>50.264285714</v>
+      </c>
+      <c r="H107" t="n">
         <v>27</v>
-      </c>
-      <c r="H107" t="n">
-        <v>50.264285714</v>
       </c>
     </row>
     <row r="108">
@@ -3451,19 +3451,19 @@
         </is>
       </c>
       <c r="D108" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E108" t="n">
         <v>-0.001414245312102238</v>
-      </c>
-      <c r="E108" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F108" t="n">
         <v>3</v>
       </c>
       <c r="G108" t="n">
+        <v>46.3</v>
+      </c>
+      <c r="H108" t="n">
         <v>33</v>
-      </c>
-      <c r="H108" t="n">
-        <v>46.3</v>
       </c>
     </row>
     <row r="109">
@@ -3479,19 +3479,19 @@
         </is>
       </c>
       <c r="D109" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E109" t="n">
         <v>-0.0007213864818561709</v>
-      </c>
-      <c r="E109" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F109" t="n">
         <v>7</v>
       </c>
       <c r="G109" t="n">
+        <v>46.3</v>
+      </c>
+      <c r="H109" t="n">
         <v>35</v>
-      </c>
-      <c r="H109" t="n">
-        <v>46.3</v>
       </c>
     </row>
     <row r="110">
@@ -3507,19 +3507,19 @@
         </is>
       </c>
       <c r="D110" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E110" t="n">
         <v>0.004376896017556402</v>
-      </c>
-      <c r="E110" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F110" t="n">
         <v>42</v>
       </c>
       <c r="G110" t="n">
+        <v>46.3</v>
+      </c>
+      <c r="H110" t="n">
         <v>31</v>
-      </c>
-      <c r="H110" t="n">
-        <v>46.3</v>
       </c>
     </row>
     <row r="111">
@@ -3535,19 +3535,19 @@
         </is>
       </c>
       <c r="D111" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E111" t="n">
         <v>0.002639431139571133</v>
-      </c>
-      <c r="E111" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F111" t="n">
         <v>38</v>
       </c>
       <c r="G111" t="n">
+        <v>46.3</v>
+      </c>
+      <c r="H111" t="n">
         <v>34</v>
-      </c>
-      <c r="H111" t="n">
-        <v>46.3</v>
       </c>
     </row>
     <row r="112">
@@ -3563,19 +3563,19 @@
         </is>
       </c>
       <c r="D112" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E112" t="n">
         <v>0.0007634974224028804</v>
-      </c>
-      <c r="E112" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F112" t="n">
         <v>31</v>
       </c>
       <c r="G112" t="n">
+        <v>47.092857143</v>
+      </c>
+      <c r="H112" t="n">
         <v>39</v>
-      </c>
-      <c r="H112" t="n">
-        <v>47.092857143</v>
       </c>
     </row>
     <row r="113">
@@ -3591,19 +3591,19 @@
         </is>
       </c>
       <c r="D113" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E113" t="n">
         <v>0.002503560850889579</v>
-      </c>
-      <c r="E113" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F113" t="n">
         <v>28</v>
       </c>
       <c r="G113" t="n">
+        <v>48.15</v>
+      </c>
+      <c r="H113" t="n">
         <v>30</v>
-      </c>
-      <c r="H113" t="n">
-        <v>48.15</v>
       </c>
     </row>
     <row r="114">
@@ -3619,19 +3619,19 @@
         </is>
       </c>
       <c r="D114" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E114" t="n">
         <v>0.005358659026915535</v>
-      </c>
-      <c r="E114" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F114" t="n">
         <v>13</v>
       </c>
       <c r="G114" t="n">
+        <v>48.15</v>
+      </c>
+      <c r="H114" t="n">
         <v>25</v>
-      </c>
-      <c r="H114" t="n">
-        <v>48.15</v>
       </c>
     </row>
     <row r="115">
@@ -3647,19 +3647,19 @@
         </is>
       </c>
       <c r="D115" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E115" t="n">
         <v>0.002284018263936385</v>
-      </c>
-      <c r="E115" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F115" t="n">
         <v>17</v>
       </c>
       <c r="G115" t="n">
+        <v>48.015714286</v>
+      </c>
+      <c r="H115" t="n">
         <v>30</v>
-      </c>
-      <c r="H115" t="n">
-        <v>48.015714286</v>
       </c>
     </row>
     <row r="116">
@@ -3675,19 +3675,19 @@
         </is>
       </c>
       <c r="D116" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E116" t="n">
         <v>0.00240019628538921</v>
-      </c>
-      <c r="E116" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F116" t="n">
         <v>24</v>
       </c>
       <c r="G116" t="n">
+        <v>48.61</v>
+      </c>
+      <c r="H116" t="n">
         <v>28</v>
-      </c>
-      <c r="H116" t="n">
-        <v>48.61</v>
       </c>
     </row>
     <row r="117">
@@ -3703,19 +3703,19 @@
         </is>
       </c>
       <c r="D117" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E117" t="n">
         <v>0.02004738767318043</v>
-      </c>
-      <c r="E117" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F117" t="n">
         <v>37</v>
       </c>
       <c r="G117" t="n">
+        <v>48.61</v>
+      </c>
+      <c r="H117" t="n">
         <v>27</v>
-      </c>
-      <c r="H117" t="n">
-        <v>48.61</v>
       </c>
     </row>
     <row r="118">
@@ -3731,19 +3731,19 @@
         </is>
       </c>
       <c r="D118" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E118" t="n">
         <v>0.02484160924992753</v>
-      </c>
-      <c r="E118" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F118" t="n">
         <v>48</v>
       </c>
       <c r="G118" t="n">
+        <v>47.818571429</v>
+      </c>
+      <c r="H118" t="n">
         <v>27</v>
-      </c>
-      <c r="H118" t="n">
-        <v>47.818571429</v>
       </c>
     </row>
     <row r="119">
@@ -3759,19 +3759,19 @@
         </is>
       </c>
       <c r="D119" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E119" t="n">
         <v>0.006341762531922348</v>
-      </c>
-      <c r="E119" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F119" t="n">
         <v>24</v>
       </c>
       <c r="G119" t="n">
+        <v>49.54</v>
+      </c>
+      <c r="H119" t="n">
         <v>34</v>
-      </c>
-      <c r="H119" t="n">
-        <v>49.54</v>
       </c>
     </row>
     <row r="120">
@@ -3787,19 +3787,19 @@
         </is>
       </c>
       <c r="D120" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E120" t="n">
         <v>0.004039360578522472</v>
-      </c>
-      <c r="E120" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F120" t="n">
         <v>17</v>
       </c>
       <c r="G120" t="n">
+        <v>47.951428571</v>
+      </c>
+      <c r="H120" t="n">
         <v>25</v>
-      </c>
-      <c r="H120" t="n">
-        <v>47.951428571</v>
       </c>
     </row>
     <row r="121">
@@ -3815,19 +3815,19 @@
         </is>
       </c>
       <c r="D121" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E121" t="n">
         <v>0.003742992946637556</v>
-      </c>
-      <c r="E121" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F121" t="n">
         <v>13</v>
       </c>
       <c r="G121" t="n">
+        <v>45.568571429</v>
+      </c>
+      <c r="H121" t="n">
         <v>27</v>
-      </c>
-      <c r="H121" t="n">
-        <v>45.568571429</v>
       </c>
     </row>
     <row r="122">
@@ -3843,19 +3843,19 @@
         </is>
       </c>
       <c r="D122" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E122" t="n">
         <v>0.008440493188665873</v>
-      </c>
-      <c r="E122" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F122" t="n">
         <v>28</v>
       </c>
       <c r="G122" t="n">
+        <v>49.54</v>
+      </c>
+      <c r="H122" t="n">
         <v>20</v>
-      </c>
-      <c r="H122" t="n">
-        <v>49.54</v>
       </c>
     </row>
     <row r="123">
@@ -3871,19 +3871,19 @@
         </is>
       </c>
       <c r="D123" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E123" t="n">
         <v>0.01991904741416087</v>
-      </c>
-      <c r="E123" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F123" t="n">
         <v>18</v>
       </c>
       <c r="G123" t="n">
+        <v>62.037142857</v>
+      </c>
+      <c r="H123" t="n">
         <v>17</v>
-      </c>
-      <c r="H123" t="n">
-        <v>62.037142857</v>
       </c>
     </row>
     <row r="124">
@@ -3899,19 +3899,19 @@
         </is>
       </c>
       <c r="D124" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E124" t="n">
         <v>0.02572893309590481</v>
-      </c>
-      <c r="E124" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F124" t="n">
         <v>26</v>
       </c>
       <c r="G124" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="H124" t="n">
         <v>18</v>
-      </c>
-      <c r="H124" t="n">
-        <v>78.7</v>
       </c>
     </row>
     <row r="125">
@@ -3927,19 +3927,19 @@
         </is>
       </c>
       <c r="D125" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E125" t="n">
         <v>0.01992083323778775</v>
-      </c>
-      <c r="E125" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F125" t="n">
         <v>16</v>
       </c>
       <c r="G125" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="H125" t="n">
         <v>19</v>
-      </c>
-      <c r="H125" t="n">
-        <v>78.7</v>
       </c>
     </row>
     <row r="126">
@@ -3955,19 +3955,19 @@
         </is>
       </c>
       <c r="D126" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E126" t="n">
         <v>0.005286479339530283</v>
-      </c>
-      <c r="E126" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F126" t="n">
         <v>32</v>
       </c>
       <c r="G126" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="H126" t="n">
         <v>19</v>
-      </c>
-      <c r="H126" t="n">
-        <v>78.7</v>
       </c>
     </row>
     <row r="127">
@@ -3983,19 +3983,19 @@
         </is>
       </c>
       <c r="D127" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E127" t="n">
         <v>0.005556197629816253</v>
-      </c>
-      <c r="E127" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F127" t="n">
         <v>32</v>
       </c>
       <c r="G127" t="n">
+        <v>77.642857143</v>
+      </c>
+      <c r="H127" t="n">
         <v>23</v>
-      </c>
-      <c r="H127" t="n">
-        <v>77.642857143</v>
       </c>
     </row>
     <row r="128">
@@ -4011,19 +4011,19 @@
         </is>
       </c>
       <c r="D128" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E128" t="n">
         <v>0.01233426019797245</v>
-      </c>
-      <c r="E128" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F128" t="n">
         <v>53</v>
       </c>
       <c r="G128" t="n">
+        <v>75</v>
+      </c>
+      <c r="H128" t="n">
         <v>23</v>
-      </c>
-      <c r="H128" t="n">
-        <v>75</v>
       </c>
     </row>
     <row r="129">
@@ -4039,19 +4039,19 @@
         </is>
       </c>
       <c r="D129" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E129" t="n">
         <v>0.008415870828738934</v>
-      </c>
-      <c r="E129" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F129" t="n">
         <v>43</v>
       </c>
       <c r="G129" t="n">
+        <v>75</v>
+      </c>
+      <c r="H129" t="n">
         <v>29</v>
-      </c>
-      <c r="H129" t="n">
-        <v>75</v>
       </c>
     </row>
     <row r="130">
@@ -4067,19 +4067,19 @@
         </is>
       </c>
       <c r="D130" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E130" t="n">
         <v>0.009680382819717856</v>
-      </c>
-      <c r="E130" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F130" t="n">
         <v>71</v>
       </c>
       <c r="G130" t="n">
+        <v>65.477142857</v>
+      </c>
+      <c r="H130" t="n">
         <v>27</v>
-      </c>
-      <c r="H130" t="n">
-        <v>65.477142857</v>
       </c>
     </row>
     <row r="131">
@@ -4095,19 +4095,19 @@
         </is>
       </c>
       <c r="D131" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E131" t="n">
         <v>0.01147904732748661</v>
-      </c>
-      <c r="E131" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F131" t="n">
         <v>75</v>
       </c>
       <c r="G131" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H131" t="n">
         <v>33</v>
-      </c>
-      <c r="H131" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="132">
@@ -4123,19 +4123,19 @@
         </is>
       </c>
       <c r="D132" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E132" t="n">
         <v>0.006436357158480325</v>
-      </c>
-      <c r="E132" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F132" t="n">
         <v>22</v>
       </c>
       <c r="G132" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H132" t="n">
         <v>37</v>
-      </c>
-      <c r="H132" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="133">
@@ -4151,19 +4151,19 @@
         </is>
       </c>
       <c r="D133" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E133" t="n">
         <v>0.005210144203667675</v>
-      </c>
-      <c r="E133" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F133" t="n">
         <v>27</v>
       </c>
       <c r="G133" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H133" t="n">
         <v>27</v>
-      </c>
-      <c r="H133" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="134">
@@ -4179,19 +4179,19 @@
         </is>
       </c>
       <c r="D134" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E134" t="n">
         <v>0.03332145399187561</v>
-      </c>
-      <c r="E134" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F134" t="n">
         <v>36</v>
       </c>
       <c r="G134" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H134" t="n">
         <v>24</v>
-      </c>
-      <c r="H134" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="135">
@@ -4207,19 +4207,19 @@
         </is>
       </c>
       <c r="D135" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E135" t="n">
         <v>0.01947487679103742</v>
-      </c>
-      <c r="E135" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F135" t="n">
         <v>16</v>
       </c>
       <c r="G135" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H135" t="n">
         <v>25</v>
-      </c>
-      <c r="H135" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="136">
@@ -4235,19 +4235,19 @@
         </is>
       </c>
       <c r="D136" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E136" t="n">
         <v>0.004663629770938988</v>
-      </c>
-      <c r="E136" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F136" t="n">
         <v>23</v>
       </c>
       <c r="G136" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H136" t="n">
         <v>20</v>
-      </c>
-      <c r="H136" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="137">
@@ -4263,19 +4263,19 @@
         </is>
       </c>
       <c r="D137" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E137" t="n">
         <v>0.0005189010792343414</v>
-      </c>
-      <c r="E137" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F137" t="n">
         <v>20</v>
       </c>
       <c r="G137" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H137" t="n">
         <v>22</v>
-      </c>
-      <c r="H137" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="138">
@@ -4291,19 +4291,19 @@
         </is>
       </c>
       <c r="D138" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E138" t="n">
         <v>0.02013964665953423</v>
-      </c>
-      <c r="E138" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F138" t="n">
         <v>13</v>
       </c>
       <c r="G138" t="n">
+        <v>60.19</v>
+      </c>
+      <c r="H138" t="n">
         <v>21</v>
-      </c>
-      <c r="H138" t="n">
-        <v>60.19</v>
       </c>
     </row>
     <row r="139">
@@ -4319,19 +4319,19 @@
         </is>
       </c>
       <c r="D139" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E139" t="n">
         <v>0.01461959034616894</v>
-      </c>
-      <c r="E139" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F139" t="n">
         <v>13</v>
       </c>
       <c r="G139" t="n">
+        <v>60.19</v>
+      </c>
+      <c r="H139" t="n">
         <v>22</v>
-      </c>
-      <c r="H139" t="n">
-        <v>60.19</v>
       </c>
     </row>
     <row r="140">
@@ -4347,19 +4347,19 @@
         </is>
       </c>
       <c r="D140" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E140" t="n">
         <v>-0.001776756973831556</v>
       </c>
-      <c r="E140" t="n">
-        <v>0.0101010101010101</v>
-      </c>
       <c r="F140" t="n">
         <v>0</v>
       </c>
       <c r="G140" t="n">
+        <v>64.552857143</v>
+      </c>
+      <c r="H140" t="n">
         <v>20</v>
-      </c>
-      <c r="H140" t="n">
-        <v>64.552857143</v>
       </c>
     </row>
     <row r="141">
@@ -4375,19 +4375,19 @@
         </is>
       </c>
       <c r="D141" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E141" t="n">
         <v>0.002178137166467781</v>
-      </c>
-      <c r="E141" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F141" t="n">
         <v>9</v>
       </c>
       <c r="G141" t="n">
+        <v>66.00714285700001</v>
+      </c>
+      <c r="H141" t="n">
         <v>26</v>
-      </c>
-      <c r="H141" t="n">
-        <v>66.00714285700001</v>
       </c>
     </row>
     <row r="142">
@@ -4403,19 +4403,19 @@
         </is>
       </c>
       <c r="D142" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E142" t="n">
         <v>-0.001029795664263842</v>
-      </c>
-      <c r="E142" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F142" t="n">
         <v>10</v>
       </c>
       <c r="G142" t="n">
+        <v>65.61</v>
+      </c>
+      <c r="H142" t="n">
         <v>23</v>
-      </c>
-      <c r="H142" t="n">
-        <v>65.61</v>
       </c>
     </row>
     <row r="143">
@@ -4431,19 +4431,19 @@
         </is>
       </c>
       <c r="D143" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E143" t="n">
         <v>-0.0007323480876772109</v>
-      </c>
-      <c r="E143" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F143" t="n">
         <v>14</v>
       </c>
       <c r="G143" t="n">
+        <v>65.61</v>
+      </c>
+      <c r="H143" t="n">
         <v>18</v>
-      </c>
-      <c r="H143" t="n">
-        <v>65.61</v>
       </c>
     </row>
     <row r="144">
@@ -4459,19 +4459,19 @@
         </is>
       </c>
       <c r="D144" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E144" t="n">
         <v>0.006137471391615688</v>
-      </c>
-      <c r="E144" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F144" t="n">
         <v>54</v>
       </c>
       <c r="G144" t="n">
+        <v>69.577142857</v>
+      </c>
+      <c r="H144" t="n">
         <v>22</v>
-      </c>
-      <c r="H144" t="n">
-        <v>69.577142857</v>
       </c>
     </row>
     <row r="145">
@@ -4487,19 +4487,19 @@
         </is>
       </c>
       <c r="D145" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E145" t="n">
         <v>0.005941977381314426</v>
-      </c>
-      <c r="E145" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F145" t="n">
         <v>58</v>
       </c>
       <c r="G145" t="n">
+        <v>68.52</v>
+      </c>
+      <c r="H145" t="n">
         <v>23</v>
-      </c>
-      <c r="H145" t="n">
-        <v>68.52</v>
       </c>
     </row>
     <row r="146">
@@ -4515,19 +4515,19 @@
         </is>
       </c>
       <c r="D146" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E146" t="n">
         <v>-0.00039966739306927</v>
-      </c>
-      <c r="E146" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F146" t="n">
         <v>3</v>
       </c>
       <c r="G146" t="n">
+        <v>74.471428571</v>
+      </c>
+      <c r="H146" t="n">
         <v>25</v>
-      </c>
-      <c r="H146" t="n">
-        <v>74.471428571</v>
       </c>
     </row>
     <row r="147">
@@ -4543,19 +4543,19 @@
         </is>
       </c>
       <c r="D147" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E147" t="n">
         <v>-0.000994432806304177</v>
-      </c>
-      <c r="E147" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F147" t="n">
         <v>5</v>
       </c>
       <c r="G147" t="n">
+        <v>75</v>
+      </c>
+      <c r="H147" t="n">
         <v>21</v>
-      </c>
-      <c r="H147" t="n">
-        <v>75</v>
       </c>
     </row>
     <row r="148">
@@ -4571,19 +4571,19 @@
         </is>
       </c>
       <c r="D148" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E148" t="n">
         <v>0.00293556569940153</v>
-      </c>
-      <c r="E148" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F148" t="n">
         <v>46</v>
       </c>
       <c r="G148" t="n">
+        <v>75</v>
+      </c>
+      <c r="H148" t="n">
         <v>20</v>
-      </c>
-      <c r="H148" t="n">
-        <v>75</v>
       </c>
     </row>
     <row r="149">
@@ -4599,19 +4599,19 @@
         </is>
       </c>
       <c r="D149" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E149" t="n">
         <v>0.003769481709610888</v>
-      </c>
-      <c r="E149" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F149" t="n">
         <v>38</v>
       </c>
       <c r="G149" t="n">
+        <v>75</v>
+      </c>
+      <c r="H149" t="n">
         <v>21</v>
-      </c>
-      <c r="H149" t="n">
-        <v>75</v>
       </c>
     </row>
     <row r="150">
@@ -4627,19 +4627,19 @@
         </is>
       </c>
       <c r="D150" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E150" t="n">
         <v>0.00599894169667809</v>
-      </c>
-      <c r="E150" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F150" t="n">
         <v>4</v>
       </c>
       <c r="G150" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H150" t="n">
         <v>25</v>
-      </c>
-      <c r="H150" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="151">
@@ -4655,19 +4655,19 @@
         </is>
       </c>
       <c r="D151" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E151" t="n">
         <v>0.004807201288955304</v>
-      </c>
-      <c r="E151" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F151" t="n">
         <v>14</v>
       </c>
       <c r="G151" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="H151" t="n">
         <v>27</v>
-      </c>
-      <c r="H151" t="n">
-        <v>63.89</v>
       </c>
     </row>
     <row r="152">
@@ -4683,19 +4683,19 @@
         </is>
       </c>
       <c r="D152" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E152" t="n">
         <v>0.005146356503197043</v>
-      </c>
-      <c r="E152" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F152" t="n">
         <v>16</v>
       </c>
       <c r="G152" t="n">
+        <v>57.275714286</v>
+      </c>
+      <c r="H152" t="n">
         <v>22</v>
-      </c>
-      <c r="H152" t="n">
-        <v>57.275714286</v>
       </c>
     </row>
     <row r="153">
@@ -4711,19 +4711,19 @@
         </is>
       </c>
       <c r="D153" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E153" t="n">
         <v>0.04111699799204318</v>
-      </c>
-      <c r="E153" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F153" t="n">
         <v>29</v>
       </c>
       <c r="G153" t="n">
+        <v>54.63</v>
+      </c>
+      <c r="H153" t="n">
         <v>21</v>
-      </c>
-      <c r="H153" t="n">
-        <v>54.63</v>
       </c>
     </row>
     <row r="154">
@@ -4739,19 +4739,19 @@
         </is>
       </c>
       <c r="D154" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E154" t="n">
         <v>0.03006537557191363</v>
-      </c>
-      <c r="E154" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F154" t="n">
         <v>35</v>
       </c>
       <c r="G154" t="n">
+        <v>54.63</v>
+      </c>
+      <c r="H154" t="n">
         <v>24</v>
-      </c>
-      <c r="H154" t="n">
-        <v>54.63</v>
       </c>
     </row>
     <row r="155">
@@ -4767,19 +4767,19 @@
         </is>
       </c>
       <c r="D155" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E155" t="n">
         <v>0.004756968971478957</v>
-      </c>
-      <c r="E155" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F155" t="n">
         <v>25</v>
       </c>
       <c r="G155" t="n">
+        <v>54.63</v>
+      </c>
+      <c r="H155" t="n">
         <v>26</v>
-      </c>
-      <c r="H155" t="n">
-        <v>54.63</v>
       </c>
     </row>
     <row r="156">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="D156" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E156" t="n">
         <v>0.006471816106636408</v>
-      </c>
-      <c r="E156" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F156" t="n">
         <v>51</v>
       </c>
       <c r="G156" t="n">
+        <v>53.571428571</v>
+      </c>
+      <c r="H156" t="n">
         <v>20</v>
-      </c>
-      <c r="H156" t="n">
-        <v>53.571428571</v>
       </c>
     </row>
     <row r="157">
@@ -4823,19 +4823,19 @@
         </is>
       </c>
       <c r="D157" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E157" t="n">
         <v>0.003759315811925113</v>
-      </c>
-      <c r="E157" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F157" t="n">
         <v>57</v>
       </c>
       <c r="G157" t="n">
+        <v>47.22</v>
+      </c>
+      <c r="H157" t="n">
         <v>21</v>
-      </c>
-      <c r="H157" t="n">
-        <v>47.22</v>
       </c>
     </row>
     <row r="158">
@@ -4851,19 +4851,19 @@
         </is>
       </c>
       <c r="D158" t="n">
+        <v>0.0101010101010101</v>
+      </c>
+      <c r="E158" t="n">
         <v>0.001598669572276741</v>
-      </c>
-      <c r="E158" t="n">
-        <v>0.0101010101010101</v>
       </c>
       <c r="F158" t="n">
         <v>13</v>
       </c>
       <c r="G158" t="n">
+        <v>46.227142857</v>
+      </c>
+      <c r="H158" t="n">
         <v>31</v>
-      </c>
-      <c r="H158" t="n">
-        <v>46.227142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>